<commit_message>
Added last part of the inputs file. Check to see if it's not easier to just do a left joint between scenario_file and pop_proj_processed
</commit_message>
<xml_diff>
--- a/data/ARM-Microsimulation/ARM_MacroScenarioInformation.xlsx
+++ b/data/ARM-Microsimulation/ARM_MacroScenarioInformation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\armenia-ccdr\data\ARM-Microsimulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renato\GitHub\armenia-ccdr\data\ARM-Microsimulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C2148E-FE3C-46E1-A59B-F146D2E45B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A05D9A9-4905-42D9-BF23-3F2BE69A116B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-20760" yWindow="1320" windowWidth="21555" windowHeight="11295" xr2:uid="{66FC96EB-762B-4856-BAC6-F6820D271721}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12549" xr2:uid="{66FC96EB-762B-4856-BAC6-F6820D271721}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="6" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>working_age_population_pp</t>
   </si>
   <si>
-    <t>populaton_m</t>
-  </si>
-  <si>
     <t>gdp_lcu</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>employment_m</t>
+  </si>
+  <si>
+    <t>population_m</t>
   </si>
 </sst>
 </file>
@@ -141,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -464,60 +464,60 @@
   <dimension ref="A1:BM40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="10" width="8.7109375" style="1"/>
-    <col min="11" max="11" width="9.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="1"/>
-    <col min="13" max="13" width="11.5703125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="10" width="8.69140625" style="1"/>
+    <col min="11" max="11" width="9.69140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.69140625" style="1"/>
+    <col min="13" max="13" width="11.53515625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.69140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="32.15" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>2022</v>
       </c>
@@ -596,7 +596,7 @@
       <c r="AY2" s="2"/>
       <c r="AZ2" s="2"/>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2023</v>
@@ -638,7 +638,7 @@
         <v>5967.7450000000008</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A39" si="0">A3+1</f>
         <v>2024</v>
@@ -680,7 +680,7 @@
         <v>6148.8160000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -722,7 +722,7 @@
         <v>6374.7150000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -764,7 +764,7 @@
         <v>6584.2939999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>2027</v>
@@ -806,7 +806,7 @@
         <v>6809.4750000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>2028</v>
@@ -848,7 +848,7 @@
         <v>7049.0550000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>2029</v>
@@ -890,7 +890,7 @@
         <v>7302.5249999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>2030</v>
@@ -932,7 +932,7 @@
         <v>7565.5840000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>2031</v>
@@ -974,7 +974,7 @@
         <v>7843.4979999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>2032</v>
@@ -1016,7 +1016,7 @@
         <v>8145.8770000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>2033</v>
@@ -1058,7 +1058,7 @@
         <v>8464.3050000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>2034</v>
@@ -1100,7 +1100,7 @@
         <v>8798.1659999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>2035</v>
@@ -1142,7 +1142,7 @@
         <v>9150.8940000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>2036</v>
@@ -1184,7 +1184,7 @@
         <v>9514.4719999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>2037</v>
@@ -1226,7 +1226,7 @@
         <v>9898.6460000000006</v>
       </c>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>2038</v>
@@ -1268,7 +1268,7 @@
         <v>10302.578000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>2039</v>
@@ -1310,7 +1310,7 @@
         <v>10733.445</v>
       </c>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>2040</v>
@@ -1352,7 +1352,7 @@
         <v>11192.293000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>2041</v>
@@ -1394,7 +1394,7 @@
         <v>11670.29</v>
       </c>
     </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>2042</v>
@@ -1443,7 +1443,7 @@
       <c r="AX22" s="3"/>
       <c r="BM22" s="3"/>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>2043</v>
@@ -1495,7 +1495,7 @@
       <c r="AI23" s="3"/>
       <c r="BM23" s="3"/>
     </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>2044</v>
@@ -1539,7 +1539,7 @@
       <c r="AI24" s="3"/>
       <c r="BM24" s="3"/>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>2045</v>
@@ -1583,7 +1583,7 @@
       <c r="AI25" s="3"/>
       <c r="BM25" s="3"/>
     </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>2046</v>
@@ -1625,7 +1625,7 @@
         <v>14327.564999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>2047</v>
@@ -1667,7 +1667,7 @@
         <v>14916.397000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>2048</v>
@@ -1709,7 +1709,7 @@
         <v>15522.626</v>
       </c>
     </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>2049</v>
@@ -1751,7 +1751,7 @@
         <v>16140.41</v>
       </c>
     </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>2050</v>
@@ -1793,7 +1793,7 @@
         <v>16776.868999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>2051</v>
@@ -1835,7 +1835,7 @@
         <v>17449.68</v>
       </c>
     </row>
-    <row r="32" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>2052</v>
@@ -1877,7 +1877,7 @@
         <v>18152.689999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>2053</v>
@@ -1919,7 +1919,7 @@
         <v>18878.41</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>2054</v>
@@ -1961,7 +1961,7 @@
         <v>19625.718000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>2055</v>
@@ -2003,7 +2003,7 @@
         <v>20376.348000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>2056</v>
@@ -2045,7 +2045,7 @@
         <v>21142.074999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>2057</v>
@@ -2087,7 +2087,7 @@
         <v>21940.457999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>2058</v>
@@ -2129,7 +2129,7 @@
         <v>22798.813000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>2059</v>
@@ -2171,7 +2171,7 @@
         <v>23733.623</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" s="1">
         <f>A39+1</f>
         <v>2060</v>

</xml_diff>

<commit_message>
Reweighting and labor heat stress
</commit_message>
<xml_diff>
--- a/data/ARM-Microsimulation/ARM_MacroScenarioInformation.xlsx
+++ b/data/ARM-Microsimulation/ARM_MacroScenarioInformation.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\armenia-ccdr\data\ARM-Microsimulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577EDACF-5665-46BD-8D74-0BE97407F20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61182F99-B707-4C19-9399-ABEDB0B1814B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{66FC96EB-762B-4856-BAC6-F6820D271721}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="8" r:id="rId1"/>
+    <sheet name="Dry-hot scenario" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -325,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -385,6 +386,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -703,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE53816-8752-4CE9-AC5C-A9E2E6E89CC8}">
   <dimension ref="A1:AT41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AU2" sqref="AU2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6345,4 +6367,4441 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A13C2AC-5F64-41F2-8EA5-531D9248B044}">
+  <dimension ref="A1:AT41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="27"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="31"/>
+    </row>
+    <row r="2" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AQ2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AS2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT2" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>45426</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C3" s="3">
+        <v>8501.44</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2.78</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.84551</v>
+      </c>
+      <c r="F3">
+        <v>48.305300000000003</v>
+      </c>
+      <c r="G3">
+        <v>304.50700000000001</v>
+      </c>
+      <c r="H3">
+        <v>444.30700000000002</v>
+      </c>
+      <c r="I3">
+        <v>337.58199999999999</v>
+      </c>
+      <c r="J3">
+        <v>250</v>
+      </c>
+      <c r="K3">
+        <v>243.90000000000003</v>
+      </c>
+      <c r="L3">
+        <v>640.80999999999995</v>
+      </c>
+      <c r="M3">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="N3">
+        <v>5.16</v>
+      </c>
+      <c r="O3">
+        <v>1.24</v>
+      </c>
+      <c r="P3">
+        <v>2.9</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>1.0363989290913931</v>
+      </c>
+      <c r="R3" s="14">
+        <v>3.9239892837183099</v>
+      </c>
+      <c r="S3" s="14">
+        <v>3.2458317434917903</v>
+      </c>
+      <c r="T3" s="2">
+        <v>889.51</v>
+      </c>
+      <c r="U3" s="2">
+        <v>2148.83</v>
+      </c>
+      <c r="V3" s="2">
+        <v>4487.13</v>
+      </c>
+      <c r="W3" s="2">
+        <v>1</v>
+      </c>
+      <c r="X3" s="15">
+        <v>905.85710000000006</v>
+      </c>
+      <c r="Y3" s="15">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="15">
+        <v>5665.8460000000005</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AM3">
+        <v>1</v>
+      </c>
+      <c r="AN3">
+        <v>1</v>
+      </c>
+      <c r="AO3">
+        <v>1</v>
+      </c>
+      <c r="AP3">
+        <v>1</v>
+      </c>
+      <c r="AQ3">
+        <v>1</v>
+      </c>
+      <c r="AR3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
+        <v>1</v>
+      </c>
+      <c r="AT3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2">
+        <f>B3+1</f>
+        <v>2023</v>
+      </c>
+      <c r="C4" s="3">
+        <v>8709.19</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2.78</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.8309500000000001</v>
+      </c>
+      <c r="F4">
+        <v>47.990099999999998</v>
+      </c>
+      <c r="G4">
+        <v>301.93900000000002</v>
+      </c>
+      <c r="H4">
+        <v>444.33</v>
+      </c>
+      <c r="I4">
+        <v>335.64299999999997</v>
+      </c>
+      <c r="J4">
+        <v>247.33</v>
+      </c>
+      <c r="K4">
+        <v>252.15</v>
+      </c>
+      <c r="L4">
+        <v>633.23</v>
+      </c>
+      <c r="M4">
+        <v>4.13</v>
+      </c>
+      <c r="N4">
+        <v>5.17</v>
+      </c>
+      <c r="O4">
+        <v>1.3</v>
+      </c>
+      <c r="P4">
+        <v>2.96</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>1.0820551807357361</v>
+      </c>
+      <c r="R4" s="14">
+        <v>4.0074416873321637</v>
+      </c>
+      <c r="S4" s="14">
+        <v>3.2901141631719582</v>
+      </c>
+      <c r="T4" s="2">
+        <v>933.87</v>
+      </c>
+      <c r="U4" s="2">
+        <v>2283.89</v>
+      </c>
+      <c r="V4" s="2">
+        <v>4557.46</v>
+      </c>
+      <c r="W4" s="2">
+        <v>1</v>
+      </c>
+      <c r="X4" s="15">
+        <v>940.08110000000011</v>
+      </c>
+      <c r="Y4" s="15">
+        <v>1.0145559165292057</v>
+      </c>
+      <c r="Z4" s="15">
+        <v>5837.4189999999999</v>
+      </c>
+      <c r="AA4">
+        <v>1.04376</v>
+      </c>
+      <c r="AB4">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="AC4">
+        <v>1.04538</v>
+      </c>
+      <c r="AD4">
+        <v>1.0455399999999999</v>
+      </c>
+      <c r="AE4">
+        <v>1.0439799999999999</v>
+      </c>
+      <c r="AF4">
+        <v>1.04403</v>
+      </c>
+      <c r="AG4">
+        <v>1.0440700000000001</v>
+      </c>
+      <c r="AH4">
+        <v>1.04495</v>
+      </c>
+      <c r="AI4">
+        <v>1.04451</v>
+      </c>
+      <c r="AJ4">
+        <v>1.04579</v>
+      </c>
+      <c r="AK4">
+        <v>0.99941599999999997</v>
+      </c>
+      <c r="AL4">
+        <v>0.99970000000000003</v>
+      </c>
+      <c r="AM4">
+        <v>1.0001899999999999</v>
+      </c>
+      <c r="AN4">
+        <v>1.0008699999999999</v>
+      </c>
+      <c r="AO4">
+        <v>1.00082</v>
+      </c>
+      <c r="AP4">
+        <v>1.0007900000000001</v>
+      </c>
+      <c r="AQ4">
+        <v>1.00116</v>
+      </c>
+      <c r="AR4">
+        <v>1.0014099999999999</v>
+      </c>
+      <c r="AS4">
+        <v>1.0024500000000001</v>
+      </c>
+      <c r="AT4">
+        <v>1.00343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2">
+        <f t="shared" ref="B5:B31" si="0">B4+1</f>
+        <v>2024</v>
+      </c>
+      <c r="C5" s="3">
+        <v>9010.5499999999993</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.78</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.8187199999999999</v>
+      </c>
+      <c r="F5">
+        <v>48.087299999999999</v>
+      </c>
+      <c r="G5">
+        <v>302.63499999999999</v>
+      </c>
+      <c r="H5">
+        <v>444.423</v>
+      </c>
+      <c r="I5">
+        <v>335.54199999999997</v>
+      </c>
+      <c r="J5">
+        <v>248.18</v>
+      </c>
+      <c r="K5">
+        <v>251.64</v>
+      </c>
+      <c r="L5">
+        <v>634.39</v>
+      </c>
+      <c r="M5">
+        <v>4.32</v>
+      </c>
+      <c r="N5">
+        <v>5.42</v>
+      </c>
+      <c r="O5">
+        <v>1.35</v>
+      </c>
+      <c r="P5">
+        <v>3.06</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>1.123776289876566</v>
+      </c>
+      <c r="R5" s="14">
+        <v>4.1574219192956612</v>
+      </c>
+      <c r="S5" s="14">
+        <v>3.4374826733284931</v>
+      </c>
+      <c r="T5" s="2">
+        <v>968.78</v>
+      </c>
+      <c r="U5" s="2">
+        <v>2355.4499999999998</v>
+      </c>
+      <c r="V5" s="2">
+        <v>4735.49</v>
+      </c>
+      <c r="W5" s="2">
+        <v>1</v>
+      </c>
+      <c r="X5" s="15">
+        <v>975.81670000000008</v>
+      </c>
+      <c r="Y5" s="15">
+        <v>1.0170757722041694</v>
+      </c>
+      <c r="Z5" s="15">
+        <v>6062.8590000000004</v>
+      </c>
+      <c r="AA5">
+        <v>1.0562199999999999</v>
+      </c>
+      <c r="AB5">
+        <v>1.05688</v>
+      </c>
+      <c r="AC5">
+        <v>1.0572299999999999</v>
+      </c>
+      <c r="AD5">
+        <v>1.05762</v>
+      </c>
+      <c r="AE5">
+        <v>1.05559</v>
+      </c>
+      <c r="AF5">
+        <v>1.0559400000000001</v>
+      </c>
+      <c r="AG5">
+        <v>1.0557000000000001</v>
+      </c>
+      <c r="AH5">
+        <v>1.0567500000000001</v>
+      </c>
+      <c r="AI5">
+        <v>1.0560099999999999</v>
+      </c>
+      <c r="AJ5">
+        <v>1.05765</v>
+      </c>
+      <c r="AK5">
+        <v>0.99235700000000004</v>
+      </c>
+      <c r="AL5">
+        <v>0.99285800000000002</v>
+      </c>
+      <c r="AM5">
+        <v>0.99372499999999997</v>
+      </c>
+      <c r="AN5">
+        <v>0.99491700000000005</v>
+      </c>
+      <c r="AO5">
+        <v>0.99482599999999999</v>
+      </c>
+      <c r="AP5">
+        <v>0.99477199999999999</v>
+      </c>
+      <c r="AQ5">
+        <v>0.99542299999999995</v>
+      </c>
+      <c r="AR5">
+        <v>0.99587300000000001</v>
+      </c>
+      <c r="AS5">
+        <v>0.99770099999999995</v>
+      </c>
+      <c r="AT5">
+        <v>0.99943000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="C6" s="3">
+        <v>9379.7099999999991</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.78</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.8071600000000001</v>
+      </c>
+      <c r="F6">
+        <v>48.257100000000001</v>
+      </c>
+      <c r="G6">
+        <v>303.73500000000001</v>
+      </c>
+      <c r="H6">
+        <v>444.68200000000002</v>
+      </c>
+      <c r="I6">
+        <v>336.02800000000002</v>
+      </c>
+      <c r="J6">
+        <v>248.01000000000002</v>
+      </c>
+      <c r="K6">
+        <v>251.57999999999998</v>
+      </c>
+      <c r="L6">
+        <v>636.85</v>
+      </c>
+      <c r="M6">
+        <v>4.55</v>
+      </c>
+      <c r="N6">
+        <v>5.7</v>
+      </c>
+      <c r="O6">
+        <v>1.4</v>
+      </c>
+      <c r="P6">
+        <v>3.18</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>1.163813194968083</v>
+      </c>
+      <c r="R6" s="14">
+        <v>4.3311533219241953</v>
+      </c>
+      <c r="S6" s="14">
+        <v>3.6063007970299275</v>
+      </c>
+      <c r="T6" s="2">
+        <v>1003.7</v>
+      </c>
+      <c r="U6" s="2">
+        <v>2441.5500000000002</v>
+      </c>
+      <c r="V6" s="2">
+        <v>4954.41</v>
+      </c>
+      <c r="W6" s="2">
+        <v>1</v>
+      </c>
+      <c r="X6" s="15">
+        <v>1012.6039000000001</v>
+      </c>
+      <c r="Y6" s="15">
+        <v>1.0166982698122833</v>
+      </c>
+      <c r="Z6" s="15">
+        <v>6325.3310000000001</v>
+      </c>
+      <c r="AA6">
+        <v>1.0516300000000001</v>
+      </c>
+      <c r="AB6">
+        <v>1.0526500000000001</v>
+      </c>
+      <c r="AC6">
+        <v>1.0529900000000001</v>
+      </c>
+      <c r="AD6">
+        <v>1.0530600000000001</v>
+      </c>
+      <c r="AE6">
+        <v>1.05131</v>
+      </c>
+      <c r="AF6">
+        <v>1.0513600000000001</v>
+      </c>
+      <c r="AG6">
+        <v>1.0512900000000001</v>
+      </c>
+      <c r="AH6">
+        <v>1.0522199999999999</v>
+      </c>
+      <c r="AI6">
+        <v>1.0515399999999999</v>
+      </c>
+      <c r="AJ6">
+        <v>1.05254</v>
+      </c>
+      <c r="AK6">
+        <v>0.99615399999999998</v>
+      </c>
+      <c r="AL6">
+        <v>0.99649699999999997</v>
+      </c>
+      <c r="AM6">
+        <v>0.99709000000000003</v>
+      </c>
+      <c r="AN6">
+        <v>0.99790699999999999</v>
+      </c>
+      <c r="AO6">
+        <v>0.99784399999999995</v>
+      </c>
+      <c r="AP6">
+        <v>0.997807</v>
+      </c>
+      <c r="AQ6">
+        <v>0.99825299999999995</v>
+      </c>
+      <c r="AR6">
+        <v>0.99856100000000003</v>
+      </c>
+      <c r="AS6">
+        <v>0.99981200000000003</v>
+      </c>
+      <c r="AT6">
+        <v>1.0009999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="C7" s="3">
+        <v>9742.5</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.78</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.7959499999999999</v>
+      </c>
+      <c r="F7">
+        <v>48.4208</v>
+      </c>
+      <c r="G7">
+        <v>304.59800000000001</v>
+      </c>
+      <c r="H7">
+        <v>445.01799999999997</v>
+      </c>
+      <c r="I7">
+        <v>336.52600000000001</v>
+      </c>
+      <c r="J7">
+        <v>247.56</v>
+      </c>
+      <c r="K7">
+        <v>250.87</v>
+      </c>
+      <c r="L7">
+        <v>640.25</v>
+      </c>
+      <c r="M7">
+        <v>4.76</v>
+      </c>
+      <c r="N7">
+        <v>5.95</v>
+      </c>
+      <c r="O7">
+        <v>1.44</v>
+      </c>
+      <c r="P7">
+        <v>3.3</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>1.2018558628394909</v>
+      </c>
+      <c r="R7" s="14">
+        <v>4.4894499954442555</v>
+      </c>
+      <c r="S7" s="14">
+        <v>3.7627935726262982</v>
+      </c>
+      <c r="T7" s="2">
+        <v>1039.3900000000001</v>
+      </c>
+      <c r="U7" s="2">
+        <v>2498.11</v>
+      </c>
+      <c r="V7" s="2">
+        <v>5170.8100000000004</v>
+      </c>
+      <c r="W7" s="2">
+        <v>1</v>
+      </c>
+      <c r="X7" s="15">
+        <v>1050.3194000000001</v>
+      </c>
+      <c r="Y7" s="15">
+        <v>1.0157715045552815</v>
+      </c>
+      <c r="Z7" s="15">
+        <v>6568.2</v>
+      </c>
+      <c r="AA7">
+        <v>1.0497700000000001</v>
+      </c>
+      <c r="AB7">
+        <v>1.0508999999999999</v>
+      </c>
+      <c r="AC7">
+        <v>1.05122</v>
+      </c>
+      <c r="AD7">
+        <v>1.0511200000000001</v>
+      </c>
+      <c r="AE7">
+        <v>1.04942</v>
+      </c>
+      <c r="AF7">
+        <v>1.04932</v>
+      </c>
+      <c r="AG7">
+        <v>1.0493300000000001</v>
+      </c>
+      <c r="AH7">
+        <v>1.0502400000000001</v>
+      </c>
+      <c r="AI7">
+        <v>1.04952</v>
+      </c>
+      <c r="AJ7">
+        <v>1.0503199999999999</v>
+      </c>
+      <c r="AK7">
+        <v>1.01627</v>
+      </c>
+      <c r="AL7">
+        <v>1.0177</v>
+      </c>
+      <c r="AM7">
+        <v>1.0201800000000001</v>
+      </c>
+      <c r="AN7">
+        <v>1.02359</v>
+      </c>
+      <c r="AO7">
+        <v>1.0233300000000001</v>
+      </c>
+      <c r="AP7">
+        <v>1.0231699999999999</v>
+      </c>
+      <c r="AQ7">
+        <v>1.0250300000000001</v>
+      </c>
+      <c r="AR7">
+        <v>1.0263199999999999</v>
+      </c>
+      <c r="AS7">
+        <v>1.0315399999999999</v>
+      </c>
+      <c r="AT7">
+        <v>1.0364800000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10102.799999999999</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.77</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.78851</v>
+      </c>
+      <c r="F8">
+        <v>48.631399999999999</v>
+      </c>
+      <c r="G8">
+        <v>305.79000000000002</v>
+      </c>
+      <c r="H8">
+        <v>446.233</v>
+      </c>
+      <c r="I8">
+        <v>337.43299999999999</v>
+      </c>
+      <c r="J8">
+        <v>248.3</v>
+      </c>
+      <c r="K8">
+        <v>250.32</v>
+      </c>
+      <c r="L8">
+        <v>644.15000000000009</v>
+      </c>
+      <c r="M8">
+        <v>4.96</v>
+      </c>
+      <c r="N8">
+        <v>6.18</v>
+      </c>
+      <c r="O8">
+        <v>1.49</v>
+      </c>
+      <c r="P8">
+        <v>3.4</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>1.2423572585638694</v>
+      </c>
+      <c r="R8" s="14">
+        <v>4.6364104316205195</v>
+      </c>
+      <c r="S8" s="14">
+        <v>3.9092670230572968</v>
+      </c>
+      <c r="T8" s="2">
+        <v>1079.24</v>
+      </c>
+      <c r="U8" s="2">
+        <v>2552.9899999999998</v>
+      </c>
+      <c r="V8" s="2">
+        <v>5383.4</v>
+      </c>
+      <c r="W8" s="2">
+        <v>1</v>
+      </c>
+      <c r="X8" s="15">
+        <v>1090.0609999999999</v>
+      </c>
+      <c r="Y8" s="15">
+        <v>1.0158034644166221</v>
+      </c>
+      <c r="Z8" s="15">
+        <v>6811.7759999999998</v>
+      </c>
+      <c r="AA8">
+        <v>1.05318</v>
+      </c>
+      <c r="AB8">
+        <v>1.05426</v>
+      </c>
+      <c r="AC8">
+        <v>1.0545899999999999</v>
+      </c>
+      <c r="AD8">
+        <v>1.0545899999999999</v>
+      </c>
+      <c r="AE8">
+        <v>1.05267</v>
+      </c>
+      <c r="AF8">
+        <v>1.0526800000000001</v>
+      </c>
+      <c r="AG8">
+        <v>1.0526</v>
+      </c>
+      <c r="AH8">
+        <v>1.0536000000000001</v>
+      </c>
+      <c r="AI8">
+        <v>1.0528</v>
+      </c>
+      <c r="AJ8">
+        <v>1.05385</v>
+      </c>
+      <c r="AK8">
+        <v>1.0354099999999999</v>
+      </c>
+      <c r="AL8">
+        <v>1.0379499999999999</v>
+      </c>
+      <c r="AM8">
+        <v>1.04234</v>
+      </c>
+      <c r="AN8">
+        <v>1.0483899999999999</v>
+      </c>
+      <c r="AO8">
+        <v>1.04792</v>
+      </c>
+      <c r="AP8">
+        <v>1.04765</v>
+      </c>
+      <c r="AQ8">
+        <v>1.0509500000000001</v>
+      </c>
+      <c r="AR8">
+        <v>1.0532300000000001</v>
+      </c>
+      <c r="AS8">
+        <v>1.0625</v>
+      </c>
+      <c r="AT8">
+        <v>1.0712600000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="C9" s="3">
+        <v>10482.5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.77</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.7847900000000001</v>
+      </c>
+      <c r="F9">
+        <v>48.910200000000003</v>
+      </c>
+      <c r="G9">
+        <v>307.38900000000001</v>
+      </c>
+      <c r="H9">
+        <v>448.04599999999999</v>
+      </c>
+      <c r="I9">
+        <v>338.91300000000001</v>
+      </c>
+      <c r="J9">
+        <v>248.79</v>
+      </c>
+      <c r="K9">
+        <v>250.43</v>
+      </c>
+      <c r="L9">
+        <v>649.13</v>
+      </c>
+      <c r="M9">
+        <v>5.15</v>
+      </c>
+      <c r="N9">
+        <v>6.4</v>
+      </c>
+      <c r="O9">
+        <v>1.53</v>
+      </c>
+      <c r="P9">
+        <v>3.51</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>1.2780000135780094</v>
+      </c>
+      <c r="R9" s="14">
+        <v>4.7739375082328879</v>
+      </c>
+      <c r="S9" s="14">
+        <v>4.0469109528486733</v>
+      </c>
+      <c r="T9" s="2">
+        <v>1122.76</v>
+      </c>
+      <c r="U9" s="2">
+        <v>2611.81</v>
+      </c>
+      <c r="V9" s="2">
+        <v>5604.5</v>
+      </c>
+      <c r="W9" s="2">
+        <v>1</v>
+      </c>
+      <c r="X9" s="15">
+        <v>1131.9377999999999</v>
+      </c>
+      <c r="Y9" s="15">
+        <v>1.0160590992463667</v>
+      </c>
+      <c r="Z9" s="15">
+        <v>7065.6390000000001</v>
+      </c>
+      <c r="AA9">
+        <v>1.0578399999999999</v>
+      </c>
+      <c r="AB9">
+        <v>1.05904</v>
+      </c>
+      <c r="AC9">
+        <v>1.05942</v>
+      </c>
+      <c r="AD9">
+        <v>1.05955</v>
+      </c>
+      <c r="AE9">
+        <v>1.05735</v>
+      </c>
+      <c r="AF9">
+        <v>1.05748</v>
+      </c>
+      <c r="AG9">
+        <v>1.05732</v>
+      </c>
+      <c r="AH9">
+        <v>1.0584499999999999</v>
+      </c>
+      <c r="AI9">
+        <v>1.0576099999999999</v>
+      </c>
+      <c r="AJ9">
+        <v>1.0590299999999999</v>
+      </c>
+      <c r="AK9">
+        <v>1.0540700000000001</v>
+      </c>
+      <c r="AL9">
+        <v>1.0577000000000001</v>
+      </c>
+      <c r="AM9">
+        <v>1.0639799999999999</v>
+      </c>
+      <c r="AN9">
+        <v>1.07263</v>
+      </c>
+      <c r="AO9">
+        <v>1.0719700000000001</v>
+      </c>
+      <c r="AP9">
+        <v>1.07158</v>
+      </c>
+      <c r="AQ9">
+        <v>1.0763</v>
+      </c>
+      <c r="AR9">
+        <v>1.0795600000000001</v>
+      </c>
+      <c r="AS9">
+        <v>1.0928100000000001</v>
+      </c>
+      <c r="AT9">
+        <v>1.10534</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10895.3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.76</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.7845599999999999</v>
+      </c>
+      <c r="F10">
+        <v>49.279600000000002</v>
+      </c>
+      <c r="G10">
+        <v>309.54000000000002</v>
+      </c>
+      <c r="H10">
+        <v>450.61900000000003</v>
+      </c>
+      <c r="I10">
+        <v>341.084</v>
+      </c>
+      <c r="J10">
+        <v>249.29</v>
+      </c>
+      <c r="K10">
+        <v>251.16000000000003</v>
+      </c>
+      <c r="L10">
+        <v>655.39</v>
+      </c>
+      <c r="M10">
+        <v>5.35</v>
+      </c>
+      <c r="N10">
+        <v>6.61</v>
+      </c>
+      <c r="O10">
+        <v>1.58</v>
+      </c>
+      <c r="P10">
+        <v>3.62</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>1.3113244208962052</v>
+      </c>
+      <c r="R10" s="14">
+        <v>4.9115138639160429</v>
+      </c>
+      <c r="S10" s="14">
+        <v>4.1845115569448215</v>
+      </c>
+      <c r="T10" s="2">
+        <v>1164.8900000000001</v>
+      </c>
+      <c r="U10" s="2">
+        <v>2678.74</v>
+      </c>
+      <c r="V10" s="2">
+        <v>5843.94</v>
+      </c>
+      <c r="W10" s="2">
+        <v>1</v>
+      </c>
+      <c r="X10" s="15">
+        <v>1176.008</v>
+      </c>
+      <c r="Y10" s="15">
+        <v>1.0153521381544959</v>
+      </c>
+      <c r="Z10" s="15">
+        <v>7336.293999999999</v>
+      </c>
+      <c r="AA10">
+        <v>1.05768</v>
+      </c>
+      <c r="AB10">
+        <v>1.05891</v>
+      </c>
+      <c r="AC10">
+        <v>1.0592999999999999</v>
+      </c>
+      <c r="AD10">
+        <v>1.05948</v>
+      </c>
+      <c r="AE10">
+        <v>1.05718</v>
+      </c>
+      <c r="AF10">
+        <v>1.0573699999999999</v>
+      </c>
+      <c r="AG10">
+        <v>1.0571600000000001</v>
+      </c>
+      <c r="AH10">
+        <v>1.05833</v>
+      </c>
+      <c r="AI10">
+        <v>1.05749</v>
+      </c>
+      <c r="AJ10">
+        <v>1.05911</v>
+      </c>
+      <c r="AK10">
+        <v>1.0725199999999999</v>
+      </c>
+      <c r="AL10">
+        <v>1.07721</v>
+      </c>
+      <c r="AM10">
+        <v>1.0853200000000001</v>
+      </c>
+      <c r="AN10">
+        <v>1.09649</v>
+      </c>
+      <c r="AO10">
+        <v>1.0956300000000001</v>
+      </c>
+      <c r="AP10">
+        <v>1.0951299999999999</v>
+      </c>
+      <c r="AQ10">
+        <v>1.1012200000000001</v>
+      </c>
+      <c r="AR10">
+        <v>1.1054299999999999</v>
+      </c>
+      <c r="AS10">
+        <v>1.1225499999999999</v>
+      </c>
+      <c r="AT10">
+        <v>1.13873</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="C11" s="3">
+        <v>11262.6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2.76</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.78637</v>
+      </c>
+      <c r="F11">
+        <v>49.624299999999998</v>
+      </c>
+      <c r="G11">
+        <v>311.63400000000001</v>
+      </c>
+      <c r="H11">
+        <v>453.65300000000002</v>
+      </c>
+      <c r="I11">
+        <v>343.11799999999999</v>
+      </c>
+      <c r="J11">
+        <v>251.53</v>
+      </c>
+      <c r="K11">
+        <v>251.44</v>
+      </c>
+      <c r="L11">
+        <v>661.05</v>
+      </c>
+      <c r="M11">
+        <v>5.5</v>
+      </c>
+      <c r="N11">
+        <v>6.78</v>
+      </c>
+      <c r="O11">
+        <v>1.62</v>
+      </c>
+      <c r="P11">
+        <v>3.71</v>
+      </c>
+      <c r="Q11" s="14">
+        <v>1.3492798416886056</v>
+      </c>
+      <c r="R11" s="14">
+        <v>5.0255948185939143</v>
+      </c>
+      <c r="S11" s="14">
+        <v>4.3019483543241384</v>
+      </c>
+      <c r="T11" s="2">
+        <v>1218.01</v>
+      </c>
+      <c r="U11" s="2">
+        <v>2731.57</v>
+      </c>
+      <c r="V11" s="2">
+        <v>6053.08</v>
+      </c>
+      <c r="W11" s="2">
+        <v>1</v>
+      </c>
+      <c r="X11" s="15">
+        <v>1221.8771999999999</v>
+      </c>
+      <c r="Y11" s="15">
+        <v>1.0176801882029145</v>
+      </c>
+      <c r="Z11" s="15">
+        <v>7588.6710000000003</v>
+      </c>
+      <c r="AA11">
+        <v>1.075</v>
+      </c>
+      <c r="AB11">
+        <v>1.0761000000000001</v>
+      </c>
+      <c r="AC11">
+        <v>1.0765499999999999</v>
+      </c>
+      <c r="AD11">
+        <v>1.0773699999999999</v>
+      </c>
+      <c r="AE11">
+        <v>1.0742</v>
+      </c>
+      <c r="AF11">
+        <v>1.0749299999999999</v>
+      </c>
+      <c r="AG11">
+        <v>1.07433</v>
+      </c>
+      <c r="AH11">
+        <v>1.07589</v>
+      </c>
+      <c r="AI11">
+        <v>1.0749</v>
+      </c>
+      <c r="AJ11">
+        <v>1.07769</v>
+      </c>
+      <c r="AK11">
+        <v>1.0927800000000001</v>
+      </c>
+      <c r="AL11">
+        <v>1.09846</v>
+      </c>
+      <c r="AM11">
+        <v>1.10829</v>
+      </c>
+      <c r="AN11">
+        <v>1.12181</v>
+      </c>
+      <c r="AO11">
+        <v>1.1207800000000001</v>
+      </c>
+      <c r="AP11">
+        <v>1.1201700000000001</v>
+      </c>
+      <c r="AQ11">
+        <v>1.1275500000000001</v>
+      </c>
+      <c r="AR11">
+        <v>1.1326499999999999</v>
+      </c>
+      <c r="AS11">
+        <v>1.15337</v>
+      </c>
+      <c r="AT11">
+        <v>1.1729700000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>2031</v>
+      </c>
+      <c r="C12" s="3">
+        <v>11707.5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.78884</v>
+      </c>
+      <c r="F12">
+        <v>50.038200000000003</v>
+      </c>
+      <c r="G12">
+        <v>314.02300000000002</v>
+      </c>
+      <c r="H12">
+        <v>456.70699999999999</v>
+      </c>
+      <c r="I12">
+        <v>345.6</v>
+      </c>
+      <c r="J12">
+        <v>252.01999999999998</v>
+      </c>
+      <c r="K12">
+        <v>252.66</v>
+      </c>
+      <c r="L12">
+        <v>667.81</v>
+      </c>
+      <c r="M12">
+        <v>5.69</v>
+      </c>
+      <c r="N12">
+        <v>6.99</v>
+      </c>
+      <c r="O12">
+        <v>1.66</v>
+      </c>
+      <c r="P12">
+        <v>3.81</v>
+      </c>
+      <c r="Q12" s="14">
+        <v>1.3813743095917208</v>
+      </c>
+      <c r="R12" s="14">
+        <v>5.155494065309548</v>
+      </c>
+      <c r="S12" s="14">
+        <v>4.4344343068895284</v>
+      </c>
+      <c r="T12" s="2">
+        <v>1267.79</v>
+      </c>
+      <c r="U12" s="2">
+        <v>2811.17</v>
+      </c>
+      <c r="V12" s="2">
+        <v>6313.94</v>
+      </c>
+      <c r="W12" s="2">
+        <v>1</v>
+      </c>
+      <c r="X12" s="15">
+        <v>1270.4336999999998</v>
+      </c>
+      <c r="Y12" s="15">
+        <v>1.0179490295614606</v>
+      </c>
+      <c r="Z12" s="15">
+        <v>7886.3830000000007</v>
+      </c>
+      <c r="AA12">
+        <v>1.0786</v>
+      </c>
+      <c r="AB12">
+        <v>1.0799799999999999</v>
+      </c>
+      <c r="AC12">
+        <v>1.0805100000000001</v>
+      </c>
+      <c r="AD12">
+        <v>1.08142</v>
+      </c>
+      <c r="AE12">
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="AF12">
+        <v>1.0788199999999999</v>
+      </c>
+      <c r="AG12">
+        <v>1.07819</v>
+      </c>
+      <c r="AH12">
+        <v>1.0798700000000001</v>
+      </c>
+      <c r="AI12">
+        <v>1.0789</v>
+      </c>
+      <c r="AJ12">
+        <v>1.0820700000000001</v>
+      </c>
+      <c r="AK12">
+        <v>1.1317200000000001</v>
+      </c>
+      <c r="AL12">
+        <v>1.13669</v>
+      </c>
+      <c r="AM12">
+        <v>1.1453100000000001</v>
+      </c>
+      <c r="AN12">
+        <v>1.15716</v>
+      </c>
+      <c r="AO12">
+        <v>1.1562600000000001</v>
+      </c>
+      <c r="AP12">
+        <v>1.1557200000000001</v>
+      </c>
+      <c r="AQ12">
+        <v>1.1621900000000001</v>
+      </c>
+      <c r="AR12">
+        <v>1.16666</v>
+      </c>
+      <c r="AS12">
+        <v>1.18483</v>
+      </c>
+      <c r="AT12">
+        <v>1.20201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>2032</v>
+      </c>
+      <c r="C13" s="3">
+        <v>12140.8</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.7919499999999999</v>
+      </c>
+      <c r="F13">
+        <v>50.431399999999996</v>
+      </c>
+      <c r="G13">
+        <v>316.34500000000003</v>
+      </c>
+      <c r="H13">
+        <v>459.86799999999999</v>
+      </c>
+      <c r="I13">
+        <v>347.98700000000002</v>
+      </c>
+      <c r="J13">
+        <v>253.10999999999999</v>
+      </c>
+      <c r="K13">
+        <v>253.76999999999998</v>
+      </c>
+      <c r="L13">
+        <v>674.12</v>
+      </c>
+      <c r="M13">
+        <v>5.86</v>
+      </c>
+      <c r="N13">
+        <v>7.18</v>
+      </c>
+      <c r="O13">
+        <v>1.71</v>
+      </c>
+      <c r="P13">
+        <v>3.91</v>
+      </c>
+      <c r="Q13" s="14">
+        <v>1.415293676671753</v>
+      </c>
+      <c r="R13" s="14">
+        <v>5.2777797492146314</v>
+      </c>
+      <c r="S13" s="14">
+        <v>4.5594361324992638</v>
+      </c>
+      <c r="T13" s="2">
+        <v>1322.86</v>
+      </c>
+      <c r="U13" s="2">
+        <v>2889.45</v>
+      </c>
+      <c r="V13" s="2">
+        <v>6566.44</v>
+      </c>
+      <c r="W13" s="2">
+        <v>1</v>
+      </c>
+      <c r="X13" s="15">
+        <v>1321.8308</v>
+      </c>
+      <c r="Y13" s="15">
+        <v>1.0199268727216959</v>
+      </c>
+      <c r="Z13" s="15">
+        <v>8183.4449999999997</v>
+      </c>
+      <c r="AA13">
+        <v>1.0920700000000001</v>
+      </c>
+      <c r="AB13">
+        <v>1.09354</v>
+      </c>
+      <c r="AC13">
+        <v>1.0941099999999999</v>
+      </c>
+      <c r="AD13">
+        <v>1.0953299999999999</v>
+      </c>
+      <c r="AE13">
+        <v>1.0912599999999999</v>
+      </c>
+      <c r="AF13">
+        <v>1.0923</v>
+      </c>
+      <c r="AG13">
+        <v>1.0914999999999999</v>
+      </c>
+      <c r="AH13">
+        <v>1.0934900000000001</v>
+      </c>
+      <c r="AI13">
+        <v>1.09236</v>
+      </c>
+      <c r="AJ13">
+        <v>1.0962700000000001</v>
+      </c>
+      <c r="AK13">
+        <v>1.16153</v>
+      </c>
+      <c r="AL13">
+        <v>1.16588</v>
+      </c>
+      <c r="AM13">
+        <v>1.1734199999999999</v>
+      </c>
+      <c r="AN13">
+        <v>1.1837899999999999</v>
+      </c>
+      <c r="AO13">
+        <v>1.1830000000000001</v>
+      </c>
+      <c r="AP13">
+        <v>1.1825300000000001</v>
+      </c>
+      <c r="AQ13">
+        <v>1.1881900000000001</v>
+      </c>
+      <c r="AR13">
+        <v>1.1920999999999999</v>
+      </c>
+      <c r="AS13">
+        <v>1.2079899999999999</v>
+      </c>
+      <c r="AT13">
+        <v>1.22302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>2033</v>
+      </c>
+      <c r="C14" s="3">
+        <v>12611.7</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2.74</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.7942400000000001</v>
+      </c>
+      <c r="F14">
+        <v>50.825899999999997</v>
+      </c>
+      <c r="G14">
+        <v>318.68</v>
+      </c>
+      <c r="H14">
+        <v>462.952</v>
+      </c>
+      <c r="I14">
+        <v>350.40899999999999</v>
+      </c>
+      <c r="J14">
+        <v>253.92</v>
+      </c>
+      <c r="K14">
+        <v>255.01</v>
+      </c>
+      <c r="L14">
+        <v>680.47</v>
+      </c>
+      <c r="M14">
+        <v>6.05</v>
+      </c>
+      <c r="N14">
+        <v>7.39</v>
+      </c>
+      <c r="O14">
+        <v>1.75</v>
+      </c>
+      <c r="P14">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="Q14" s="14">
+        <v>1.4510046393471123</v>
+      </c>
+      <c r="R14" s="14">
+        <v>5.4148441427097707</v>
+      </c>
+      <c r="S14" s="14">
+        <v>4.6971923344134172</v>
+      </c>
+      <c r="T14" s="2">
+        <v>1377.29</v>
+      </c>
+      <c r="U14" s="2">
+        <v>2977.32</v>
+      </c>
+      <c r="V14" s="2">
+        <v>6841.37</v>
+      </c>
+      <c r="W14" s="2">
+        <v>1</v>
+      </c>
+      <c r="X14" s="15">
+        <v>1375.5828999999999</v>
+      </c>
+      <c r="Y14" s="15">
+        <v>1.0209224382536908</v>
+      </c>
+      <c r="Z14" s="15">
+        <v>8502.5730000000003</v>
+      </c>
+      <c r="AA14">
+        <v>1.0999000000000001</v>
+      </c>
+      <c r="AB14">
+        <v>1.1014999999999999</v>
+      </c>
+      <c r="AC14">
+        <v>1.1021000000000001</v>
+      </c>
+      <c r="AD14">
+        <v>1.1034200000000001</v>
+      </c>
+      <c r="AE14">
+        <v>1.09897</v>
+      </c>
+      <c r="AF14">
+        <v>1.10006</v>
+      </c>
+      <c r="AG14">
+        <v>1.0992</v>
+      </c>
+      <c r="AH14">
+        <v>1.1013900000000001</v>
+      </c>
+      <c r="AI14">
+        <v>1.10015</v>
+      </c>
+      <c r="AJ14">
+        <v>1.1044799999999999</v>
+      </c>
+      <c r="AK14">
+        <v>1.18543</v>
+      </c>
+      <c r="AL14">
+        <v>1.18923</v>
+      </c>
+      <c r="AM14">
+        <v>1.19581</v>
+      </c>
+      <c r="AN14">
+        <v>1.2048700000000001</v>
+      </c>
+      <c r="AO14">
+        <v>1.20418</v>
+      </c>
+      <c r="AP14">
+        <v>1.20377</v>
+      </c>
+      <c r="AQ14">
+        <v>1.20872</v>
+      </c>
+      <c r="AR14">
+        <v>1.2121299999999999</v>
+      </c>
+      <c r="AS14">
+        <v>1.22601</v>
+      </c>
+      <c r="AT14">
+        <v>1.2391399999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>2034</v>
+      </c>
+      <c r="C15" s="3">
+        <v>13110.4</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2.73</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.7955000000000001</v>
+      </c>
+      <c r="F15">
+        <v>51.198300000000003</v>
+      </c>
+      <c r="G15">
+        <v>320.892</v>
+      </c>
+      <c r="H15">
+        <v>465.75299999999999</v>
+      </c>
+      <c r="I15">
+        <v>352.73200000000003</v>
+      </c>
+      <c r="J15">
+        <v>254.23</v>
+      </c>
+      <c r="K15">
+        <v>256.34000000000003</v>
+      </c>
+      <c r="L15">
+        <v>686.59999999999991</v>
+      </c>
+      <c r="M15">
+        <v>6.25</v>
+      </c>
+      <c r="N15">
+        <v>7.61</v>
+      </c>
+      <c r="O15">
+        <v>1.8</v>
+      </c>
+      <c r="P15">
+        <v>4.13</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>1.4857957844483394</v>
+      </c>
+      <c r="R15" s="14">
+        <v>5.559192202824681</v>
+      </c>
+      <c r="S15" s="14">
+        <v>4.8410791871098136</v>
+      </c>
+      <c r="T15" s="2">
+        <v>1434.32</v>
+      </c>
+      <c r="U15" s="2">
+        <v>3071.05</v>
+      </c>
+      <c r="V15" s="2">
+        <v>7130.19</v>
+      </c>
+      <c r="W15" s="2">
+        <v>1</v>
+      </c>
+      <c r="X15" s="15">
+        <v>1431.7413999999999</v>
+      </c>
+      <c r="Y15" s="15">
+        <v>1.0215572766033139</v>
+      </c>
+      <c r="Z15" s="15">
+        <v>8837.5079999999998</v>
+      </c>
+      <c r="AA15">
+        <v>1.10636</v>
+      </c>
+      <c r="AB15">
+        <v>1.10819</v>
+      </c>
+      <c r="AC15">
+        <v>1.1088499999999999</v>
+      </c>
+      <c r="AD15">
+        <v>1.11032</v>
+      </c>
+      <c r="AE15">
+        <v>1.10551</v>
+      </c>
+      <c r="AF15">
+        <v>1.1067199999999999</v>
+      </c>
+      <c r="AG15">
+        <v>1.1057999999999999</v>
+      </c>
+      <c r="AH15">
+        <v>1.10815</v>
+      </c>
+      <c r="AI15">
+        <v>1.1068800000000001</v>
+      </c>
+      <c r="AJ15">
+        <v>1.11165</v>
+      </c>
+      <c r="AK15">
+        <v>1.2049399999999999</v>
+      </c>
+      <c r="AL15">
+        <v>1.2082900000000001</v>
+      </c>
+      <c r="AM15">
+        <v>1.2140899999999999</v>
+      </c>
+      <c r="AN15">
+        <v>1.22207</v>
+      </c>
+      <c r="AO15">
+        <v>1.22146</v>
+      </c>
+      <c r="AP15">
+        <v>1.2211000000000001</v>
+      </c>
+      <c r="AQ15">
+        <v>1.2254499999999999</v>
+      </c>
+      <c r="AR15">
+        <v>1.2284600000000001</v>
+      </c>
+      <c r="AS15">
+        <v>1.2406900000000001</v>
+      </c>
+      <c r="AT15">
+        <v>1.2522599999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>2035</v>
+      </c>
+      <c r="C16" s="3">
+        <v>13625.9</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2.73</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.79522</v>
+      </c>
+      <c r="F16">
+        <v>51.553100000000001</v>
+      </c>
+      <c r="G16">
+        <v>323.048</v>
+      </c>
+      <c r="H16">
+        <v>468.51100000000002</v>
+      </c>
+      <c r="I16">
+        <v>354.81400000000002</v>
+      </c>
+      <c r="J16">
+        <v>255.31000000000003</v>
+      </c>
+      <c r="K16">
+        <v>257.23</v>
+      </c>
+      <c r="L16">
+        <v>692.1</v>
+      </c>
+      <c r="M16">
+        <v>6.46</v>
+      </c>
+      <c r="N16">
+        <v>7.87</v>
+      </c>
+      <c r="O16">
+        <v>1.86</v>
+      </c>
+      <c r="P16">
+        <v>4.26</v>
+      </c>
+      <c r="Q16" s="14">
+        <v>1.5293732413483694</v>
+      </c>
+      <c r="R16" s="14">
+        <v>5.7185596184190981</v>
+      </c>
+      <c r="S16" s="14">
+        <v>5.0043985524288672</v>
+      </c>
+      <c r="T16" s="2">
+        <v>1490.38</v>
+      </c>
+      <c r="U16" s="2">
+        <v>3166.63</v>
+      </c>
+      <c r="V16" s="2">
+        <v>7433.43</v>
+      </c>
+      <c r="W16" s="2">
+        <v>1</v>
+      </c>
+      <c r="X16" s="15">
+        <v>1490.2570000000001</v>
+      </c>
+      <c r="Y16" s="15">
+        <v>1.0216110247280938</v>
+      </c>
+      <c r="Z16" s="15">
+        <v>9187.0810000000001</v>
+      </c>
+      <c r="AA16">
+        <v>1.1111800000000001</v>
+      </c>
+      <c r="AB16">
+        <v>1.1127800000000001</v>
+      </c>
+      <c r="AC16">
+        <v>1.11341</v>
+      </c>
+      <c r="AD16">
+        <v>1.11521</v>
+      </c>
+      <c r="AE16">
+        <v>1.1101000000000001</v>
+      </c>
+      <c r="AF16">
+        <v>1.1115900000000001</v>
+      </c>
+      <c r="AG16">
+        <v>1.1104400000000001</v>
+      </c>
+      <c r="AH16">
+        <v>1.1129100000000001</v>
+      </c>
+      <c r="AI16">
+        <v>1.1115999999999999</v>
+      </c>
+      <c r="AJ16">
+        <v>1.11686</v>
+      </c>
+      <c r="AK16">
+        <v>1.18892</v>
+      </c>
+      <c r="AL16">
+        <v>1.1933800000000001</v>
+      </c>
+      <c r="AM16">
+        <v>1.2011099999999999</v>
+      </c>
+      <c r="AN16">
+        <v>1.2117500000000001</v>
+      </c>
+      <c r="AO16">
+        <v>1.2109399999999999</v>
+      </c>
+      <c r="AP16">
+        <v>1.2104600000000001</v>
+      </c>
+      <c r="AQ16">
+        <v>1.21627</v>
+      </c>
+      <c r="AR16">
+        <v>1.22028</v>
+      </c>
+      <c r="AS16">
+        <v>1.23658</v>
+      </c>
+      <c r="AT16">
+        <v>1.252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>2036</v>
+      </c>
+      <c r="C17" s="3">
+        <v>14198.9</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2.72</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1.7943100000000001</v>
+      </c>
+      <c r="F17">
+        <v>51.929400000000001</v>
+      </c>
+      <c r="G17">
+        <v>325.197</v>
+      </c>
+      <c r="H17">
+        <v>471.161</v>
+      </c>
+      <c r="I17">
+        <v>357.12700000000001</v>
+      </c>
+      <c r="J17">
+        <v>255.24999999999997</v>
+      </c>
+      <c r="K17">
+        <v>258.29999999999995</v>
+      </c>
+      <c r="L17">
+        <v>698.36</v>
+      </c>
+      <c r="M17">
+        <v>6.71</v>
+      </c>
+      <c r="N17">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="O17">
+        <v>1.91</v>
+      </c>
+      <c r="P17">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q17" s="14">
+        <v>1.5698108522976055</v>
+      </c>
+      <c r="R17" s="14">
+        <v>5.8918445825145014</v>
+      </c>
+      <c r="S17" s="14">
+        <v>5.1771368250395451</v>
+      </c>
+      <c r="T17" s="2">
+        <v>1543.51</v>
+      </c>
+      <c r="U17" s="2">
+        <v>3264.31</v>
+      </c>
+      <c r="V17" s="2">
+        <v>7771.06</v>
+      </c>
+      <c r="W17" s="2">
+        <v>1</v>
+      </c>
+      <c r="X17" s="15">
+        <v>1551.6674</v>
+      </c>
+      <c r="Y17" s="15">
+        <v>1.0194687159247211</v>
+      </c>
+      <c r="Z17" s="15">
+        <v>9559.5330000000013</v>
+      </c>
+      <c r="AA17">
+        <v>1.10734</v>
+      </c>
+      <c r="AB17">
+        <v>1.1087</v>
+      </c>
+      <c r="AC17">
+        <v>1.1092900000000001</v>
+      </c>
+      <c r="AD17">
+        <v>1.11117</v>
+      </c>
+      <c r="AE17">
+        <v>1.10609</v>
+      </c>
+      <c r="AF17">
+        <v>1.1076699999999999</v>
+      </c>
+      <c r="AG17">
+        <v>1.1064400000000001</v>
+      </c>
+      <c r="AH17">
+        <v>1.10887</v>
+      </c>
+      <c r="AI17">
+        <v>1.1075600000000001</v>
+      </c>
+      <c r="AJ17">
+        <v>1.11297</v>
+      </c>
+      <c r="AK17">
+        <v>1.1650799999999999</v>
+      </c>
+      <c r="AL17">
+        <v>1.16967</v>
+      </c>
+      <c r="AM17">
+        <v>1.1776</v>
+      </c>
+      <c r="AN17">
+        <v>1.1885300000000001</v>
+      </c>
+      <c r="AO17">
+        <v>1.1876899999999999</v>
+      </c>
+      <c r="AP17">
+        <v>1.1872</v>
+      </c>
+      <c r="AQ17">
+        <v>1.19316</v>
+      </c>
+      <c r="AR17">
+        <v>1.1972799999999999</v>
+      </c>
+      <c r="AS17">
+        <v>1.2140200000000001</v>
+      </c>
+      <c r="AT17">
+        <v>1.22984</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>2037</v>
+      </c>
+      <c r="C18" s="3">
+        <v>14854.8</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2.71</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1.7925599999999999</v>
+      </c>
+      <c r="F18">
+        <v>52.325699999999998</v>
+      </c>
+      <c r="G18">
+        <v>327.41800000000001</v>
+      </c>
+      <c r="H18">
+        <v>473.637</v>
+      </c>
+      <c r="I18">
+        <v>359.61799999999999</v>
+      </c>
+      <c r="J18">
+        <v>254.06</v>
+      </c>
+      <c r="K18">
+        <v>259.79999999999995</v>
+      </c>
+      <c r="L18">
+        <v>705.12999999999988</v>
+      </c>
+      <c r="M18">
+        <v>6.99</v>
+      </c>
+      <c r="N18">
+        <v>8.43</v>
+      </c>
+      <c r="O18">
+        <v>1.97</v>
+      </c>
+      <c r="P18">
+        <v>4.57</v>
+      </c>
+      <c r="Q18" s="14">
+        <v>1.6087934838957576</v>
+      </c>
+      <c r="R18" s="14">
+        <v>6.091172312670972</v>
+      </c>
+      <c r="S18" s="14">
+        <v>5.3730141815622465</v>
+      </c>
+      <c r="T18" s="2">
+        <v>1597.27</v>
+      </c>
+      <c r="U18" s="2">
+        <v>3382.44</v>
+      </c>
+      <c r="V18" s="2">
+        <v>8159.85</v>
+      </c>
+      <c r="W18" s="2">
+        <v>1</v>
+      </c>
+      <c r="X18" s="15">
+        <v>1615.9543999999999</v>
+      </c>
+      <c r="Y18" s="15">
+        <v>1.0160249661780245</v>
+      </c>
+      <c r="Z18" s="15">
+        <v>9979.902</v>
+      </c>
+      <c r="AA18">
+        <v>1.09148</v>
+      </c>
+      <c r="AB18">
+        <v>1.0931599999999999</v>
+      </c>
+      <c r="AC18">
+        <v>1.09378</v>
+      </c>
+      <c r="AD18">
+        <v>1.09518</v>
+      </c>
+      <c r="AE18">
+        <v>1.0906800000000001</v>
+      </c>
+      <c r="AF18">
+        <v>1.0919399999999999</v>
+      </c>
+      <c r="AG18">
+        <v>1.0909899999999999</v>
+      </c>
+      <c r="AH18">
+        <v>1.0931500000000001</v>
+      </c>
+      <c r="AI18">
+        <v>1.0920300000000001</v>
+      </c>
+      <c r="AJ18">
+        <v>1.09684</v>
+      </c>
+      <c r="AK18">
+        <v>1.1422600000000001</v>
+      </c>
+      <c r="AL18">
+        <v>1.1469199999999999</v>
+      </c>
+      <c r="AM18">
+        <v>1.1550100000000001</v>
+      </c>
+      <c r="AN18">
+        <v>1.1661300000000001</v>
+      </c>
+      <c r="AO18">
+        <v>1.1652800000000001</v>
+      </c>
+      <c r="AP18">
+        <v>1.1647799999999999</v>
+      </c>
+      <c r="AQ18">
+        <v>1.1708499999999999</v>
+      </c>
+      <c r="AR18">
+        <v>1.1750400000000001</v>
+      </c>
+      <c r="AS18">
+        <v>1.1920900000000001</v>
+      </c>
+      <c r="AT18">
+        <v>1.20821</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>2038</v>
+      </c>
+      <c r="C19" s="3">
+        <v>15480.7</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.78956</v>
+      </c>
+      <c r="F19">
+        <v>52.642800000000001</v>
+      </c>
+      <c r="G19">
+        <v>329.22399999999999</v>
+      </c>
+      <c r="H19">
+        <v>475.85300000000001</v>
+      </c>
+      <c r="I19">
+        <v>361.58100000000002</v>
+      </c>
+      <c r="J19">
+        <v>253.79</v>
+      </c>
+      <c r="K19">
+        <v>260.68</v>
+      </c>
+      <c r="L19">
+        <v>710.59999999999991</v>
+      </c>
+      <c r="M19">
+        <v>7.26</v>
+      </c>
+      <c r="N19">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="O19">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="P19">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="Q19" s="14">
+        <v>1.6537843697615342</v>
+      </c>
+      <c r="R19" s="14">
+        <v>6.2829307947384523</v>
+      </c>
+      <c r="S19" s="14">
+        <v>5.5622373534930674</v>
+      </c>
+      <c r="T19" s="2">
+        <v>1657.33</v>
+      </c>
+      <c r="U19" s="2">
+        <v>3491.56</v>
+      </c>
+      <c r="V19" s="2">
+        <v>8528.3799999999992</v>
+      </c>
+      <c r="W19" s="2">
+        <v>1</v>
+      </c>
+      <c r="X19" s="15">
+        <v>1682.8923</v>
+      </c>
+      <c r="Y19" s="15">
+        <v>1.0144824247518569</v>
+      </c>
+      <c r="Z19" s="15">
+        <v>10388.860999999999</v>
+      </c>
+      <c r="AA19">
+        <v>1.0886800000000001</v>
+      </c>
+      <c r="AB19">
+        <v>1.0903799999999999</v>
+      </c>
+      <c r="AC19">
+        <v>1.09101</v>
+      </c>
+      <c r="AD19">
+        <v>1.0923499999999999</v>
+      </c>
+      <c r="AE19">
+        <v>1.08788</v>
+      </c>
+      <c r="AF19">
+        <v>1.0891200000000001</v>
+      </c>
+      <c r="AG19">
+        <v>1.08819</v>
+      </c>
+      <c r="AH19">
+        <v>1.09033</v>
+      </c>
+      <c r="AI19">
+        <v>1.0892200000000001</v>
+      </c>
+      <c r="AJ19">
+        <v>1.0940799999999999</v>
+      </c>
+      <c r="AK19">
+        <v>1.1181700000000001</v>
+      </c>
+      <c r="AL19">
+        <v>1.1229899999999999</v>
+      </c>
+      <c r="AM19">
+        <v>1.1313299999999999</v>
+      </c>
+      <c r="AN19">
+        <v>1.1428100000000001</v>
+      </c>
+      <c r="AO19">
+        <v>1.14194</v>
+      </c>
+      <c r="AP19">
+        <v>1.1414200000000001</v>
+      </c>
+      <c r="AQ19">
+        <v>1.14768</v>
+      </c>
+      <c r="AR19">
+        <v>1.15201</v>
+      </c>
+      <c r="AS19">
+        <v>1.16961</v>
+      </c>
+      <c r="AT19">
+        <v>1.18624</v>
+      </c>
+    </row>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>2039</v>
+      </c>
+      <c r="C20" s="3">
+        <v>16150.3</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2.69</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.7862899999999999</v>
+      </c>
+      <c r="F20">
+        <v>52.956600000000002</v>
+      </c>
+      <c r="G20">
+        <v>330.995</v>
+      </c>
+      <c r="H20">
+        <v>478.00400000000002</v>
+      </c>
+      <c r="I20">
+        <v>363.56200000000001</v>
+      </c>
+      <c r="J20">
+        <v>253.16</v>
+      </c>
+      <c r="K20">
+        <v>261.71000000000004</v>
+      </c>
+      <c r="L20">
+        <v>716.15000000000009</v>
+      </c>
+      <c r="M20">
+        <v>7.53</v>
+      </c>
+      <c r="N20">
+        <v>9.02</v>
+      </c>
+      <c r="O20">
+        <v>2.1</v>
+      </c>
+      <c r="P20">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Q20" s="14">
+        <v>1.6994285809436169</v>
+      </c>
+      <c r="R20" s="14">
+        <v>6.4855442527568661</v>
+      </c>
+      <c r="S20" s="14">
+        <v>5.7605055120407167</v>
+      </c>
+      <c r="T20" s="2">
+        <v>1722.28</v>
+      </c>
+      <c r="U20" s="2">
+        <v>3610.94</v>
+      </c>
+      <c r="V20" s="2">
+        <v>8922.9699999999993</v>
+      </c>
+      <c r="W20" s="2">
+        <v>1</v>
+      </c>
+      <c r="X20" s="15">
+        <v>1753.1889000000001</v>
+      </c>
+      <c r="Y20" s="15">
+        <v>1.0131136602724218</v>
+      </c>
+      <c r="Z20" s="15">
+        <v>10826.297999999999</v>
+      </c>
+      <c r="AA20">
+        <v>1.0845800000000001</v>
+      </c>
+      <c r="AB20">
+        <v>1.0866400000000001</v>
+      </c>
+      <c r="AC20">
+        <v>1.08731</v>
+      </c>
+      <c r="AD20">
+        <v>1.0883700000000001</v>
+      </c>
+      <c r="AE20">
+        <v>1.08402</v>
+      </c>
+      <c r="AF20">
+        <v>1.0850299999999999</v>
+      </c>
+      <c r="AG20">
+        <v>1.0842799999999999</v>
+      </c>
+      <c r="AH20">
+        <v>1.0863799999999999</v>
+      </c>
+      <c r="AI20">
+        <v>1.08531</v>
+      </c>
+      <c r="AJ20">
+        <v>1.08996</v>
+      </c>
+      <c r="AK20">
+        <v>1.09395</v>
+      </c>
+      <c r="AL20">
+        <v>1.0989199999999999</v>
+      </c>
+      <c r="AM20">
+        <v>1.1075299999999999</v>
+      </c>
+      <c r="AN20">
+        <v>1.11938</v>
+      </c>
+      <c r="AO20">
+        <v>1.1184700000000001</v>
+      </c>
+      <c r="AP20">
+        <v>1.1179399999999999</v>
+      </c>
+      <c r="AQ20">
+        <v>1.1244000000000001</v>
+      </c>
+      <c r="AR20">
+        <v>1.12887</v>
+      </c>
+      <c r="AS20">
+        <v>1.1470199999999999</v>
+      </c>
+      <c r="AT20">
+        <v>1.16418</v>
+      </c>
+    </row>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>2040</v>
+      </c>
+      <c r="C21" s="3">
+        <v>16833</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2.68</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1.78159</v>
+      </c>
+      <c r="F21">
+        <v>53.213900000000002</v>
+      </c>
+      <c r="G21">
+        <v>332.42</v>
+      </c>
+      <c r="H21">
+        <v>479.74900000000002</v>
+      </c>
+      <c r="I21">
+        <v>365.22300000000001</v>
+      </c>
+      <c r="J21">
+        <v>252.29</v>
+      </c>
+      <c r="K21">
+        <v>262.55</v>
+      </c>
+      <c r="L21">
+        <v>721.05</v>
+      </c>
+      <c r="M21">
+        <v>7.81</v>
+      </c>
+      <c r="N21">
+        <v>9.32</v>
+      </c>
+      <c r="O21">
+        <v>2.16</v>
+      </c>
+      <c r="P21">
+        <v>5.07</v>
+      </c>
+      <c r="Q21" s="14">
+        <v>1.745778417656179</v>
+      </c>
+      <c r="R21" s="14">
+        <v>6.6912936896869812</v>
+      </c>
+      <c r="S21" s="14">
+        <v>5.9590648107135999</v>
+      </c>
+      <c r="T21" s="2">
+        <v>1790.54</v>
+      </c>
+      <c r="U21" s="2">
+        <v>3732.42</v>
+      </c>
+      <c r="V21" s="2">
+        <v>9322.3799999999992</v>
+      </c>
+      <c r="W21" s="2">
+        <v>1</v>
+      </c>
+      <c r="X21" s="15">
+        <v>1826.6590999999999</v>
+      </c>
+      <c r="Y21" s="15">
+        <v>1.0123357427804347</v>
+      </c>
+      <c r="Z21" s="15">
+        <v>11271.662</v>
+      </c>
+      <c r="AA21">
+        <v>1.08447</v>
+      </c>
+      <c r="AB21">
+        <v>1.0868599999999999</v>
+      </c>
+      <c r="AC21">
+        <v>1.0875699999999999</v>
+      </c>
+      <c r="AD21">
+        <v>1.0883700000000001</v>
+      </c>
+      <c r="AE21">
+        <v>1.08399</v>
+      </c>
+      <c r="AF21">
+        <v>1.0847800000000001</v>
+      </c>
+      <c r="AG21">
+        <v>1.0842000000000001</v>
+      </c>
+      <c r="AH21">
+        <v>1.08633</v>
+      </c>
+      <c r="AI21">
+        <v>1.0852200000000001</v>
+      </c>
+      <c r="AJ21">
+        <v>1.08979</v>
+      </c>
+      <c r="AK21">
+        <v>1.0825</v>
+      </c>
+      <c r="AL21">
+        <v>1.0871</v>
+      </c>
+      <c r="AM21">
+        <v>1.0950599999999999</v>
+      </c>
+      <c r="AN21">
+        <v>1.1060300000000001</v>
+      </c>
+      <c r="AO21">
+        <v>1.1051899999999999</v>
+      </c>
+      <c r="AP21">
+        <v>1.1046899999999999</v>
+      </c>
+      <c r="AQ21">
+        <v>1.1106799999999999</v>
+      </c>
+      <c r="AR21">
+        <v>1.1148100000000001</v>
+      </c>
+      <c r="AS21">
+        <v>1.13161</v>
+      </c>
+      <c r="AT21">
+        <v>1.1475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>2041</v>
+      </c>
+      <c r="C22" s="3">
+        <v>17473</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2.67</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1.7749699999999999</v>
+      </c>
+      <c r="F22">
+        <v>53.397500000000001</v>
+      </c>
+      <c r="G22">
+        <v>333.53699999999998</v>
+      </c>
+      <c r="H22">
+        <v>481.19</v>
+      </c>
+      <c r="I22">
+        <v>366.11900000000003</v>
+      </c>
+      <c r="J22">
+        <v>253.24999999999997</v>
+      </c>
+      <c r="K22">
+        <v>262.60000000000002</v>
+      </c>
+      <c r="L22">
+        <v>723.72</v>
+      </c>
+      <c r="M22">
+        <v>8.09</v>
+      </c>
+      <c r="N22">
+        <v>9.65</v>
+      </c>
+      <c r="O22">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="P22">
+        <v>5.23</v>
+      </c>
+      <c r="Q22" s="14">
+        <v>1.8065206200849124</v>
+      </c>
+      <c r="R22" s="14">
+        <v>6.8995359209054756</v>
+      </c>
+      <c r="S22" s="14">
+        <v>6.1723370466401999</v>
+      </c>
+      <c r="T22" s="2">
+        <v>1868.87</v>
+      </c>
+      <c r="U22" s="2">
+        <v>3851.26</v>
+      </c>
+      <c r="V22" s="2">
+        <v>9702.09</v>
+      </c>
+      <c r="W22" s="2">
+        <v>1</v>
+      </c>
+      <c r="X22" s="15">
+        <v>1903.2457999999999</v>
+      </c>
+      <c r="Y22" s="15">
+        <v>1.014209514321426</v>
+      </c>
+      <c r="Z22" s="15">
+        <v>11716.885</v>
+      </c>
+      <c r="AA22">
+        <v>1.0987499999999999</v>
+      </c>
+      <c r="AB22">
+        <v>1.1011500000000001</v>
+      </c>
+      <c r="AC22">
+        <v>1.10189</v>
+      </c>
+      <c r="AD22">
+        <v>1.10301</v>
+      </c>
+      <c r="AE22">
+        <v>1.0980099999999999</v>
+      </c>
+      <c r="AF22">
+        <v>1.0990599999999999</v>
+      </c>
+      <c r="AG22">
+        <v>1.0982700000000001</v>
+      </c>
+      <c r="AH22">
+        <v>1.1006800000000001</v>
+      </c>
+      <c r="AI22">
+        <v>1.09941</v>
+      </c>
+      <c r="AJ22">
+        <v>1.1046199999999999</v>
+      </c>
+      <c r="AK22">
+        <v>1.0485599999999999</v>
+      </c>
+      <c r="AL22">
+        <v>1.0533399999999999</v>
+      </c>
+      <c r="AM22">
+        <v>1.0616300000000001</v>
+      </c>
+      <c r="AN22">
+        <v>1.07304</v>
+      </c>
+      <c r="AO22">
+        <v>1.0721700000000001</v>
+      </c>
+      <c r="AP22">
+        <v>1.07165</v>
+      </c>
+      <c r="AQ22">
+        <v>1.0778799999999999</v>
+      </c>
+      <c r="AR22">
+        <v>1.0821799999999999</v>
+      </c>
+      <c r="AS22">
+        <v>1.0996699999999999</v>
+      </c>
+      <c r="AT22">
+        <v>1.1162000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>2042</v>
+      </c>
+      <c r="C23" s="3">
+        <v>18145.400000000001</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2.66</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1.7677</v>
+      </c>
+      <c r="F23">
+        <v>53.572000000000003</v>
+      </c>
+      <c r="G23">
+        <v>334.57900000000001</v>
+      </c>
+      <c r="H23">
+        <v>482.50299999999999</v>
+      </c>
+      <c r="I23">
+        <v>366.96899999999999</v>
+      </c>
+      <c r="J23">
+        <v>253.95</v>
+      </c>
+      <c r="K23">
+        <v>262.63</v>
+      </c>
+      <c r="L23">
+        <v>726.35</v>
+      </c>
+      <c r="M23">
+        <v>8.39</v>
+      </c>
+      <c r="N23">
+        <v>10.01</v>
+      </c>
+      <c r="O23">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="P23">
+        <v>5.4</v>
+      </c>
+      <c r="Q23" s="14">
+        <v>1.8692886068708823</v>
+      </c>
+      <c r="R23" s="14">
+        <v>7.1198988266522392</v>
+      </c>
+      <c r="S23" s="14">
+        <v>6.3965530046400705</v>
+      </c>
+      <c r="T23" s="2">
+        <v>1944.07</v>
+      </c>
+      <c r="U23" s="2">
+        <v>3977.32</v>
+      </c>
+      <c r="V23" s="2">
+        <v>10102.86</v>
+      </c>
+      <c r="W23" s="2">
+        <v>1</v>
+      </c>
+      <c r="X23" s="15">
+        <v>1982.8500000000001</v>
+      </c>
+      <c r="Y23" s="15">
+        <v>1.015452251433641</v>
+      </c>
+      <c r="Z23" s="15">
+        <v>12179.826000000001</v>
+      </c>
+      <c r="AA23">
+        <v>1.1099600000000001</v>
+      </c>
+      <c r="AB23">
+        <v>1.1121700000000001</v>
+      </c>
+      <c r="AC23">
+        <v>1.1128800000000001</v>
+      </c>
+      <c r="AD23">
+        <v>1.1142799999999999</v>
+      </c>
+      <c r="AE23">
+        <v>1.1087800000000001</v>
+      </c>
+      <c r="AF23">
+        <v>1.11002</v>
+      </c>
+      <c r="AG23">
+        <v>1.10904</v>
+      </c>
+      <c r="AH23">
+        <v>1.1116699999999999</v>
+      </c>
+      <c r="AI23">
+        <v>1.11022</v>
+      </c>
+      <c r="AJ23">
+        <v>1.11595</v>
+      </c>
+      <c r="AK23">
+        <v>1.0153399999999999</v>
+      </c>
+      <c r="AL23">
+        <v>1.0203100000000001</v>
+      </c>
+      <c r="AM23">
+        <v>1.0289200000000001</v>
+      </c>
+      <c r="AN23">
+        <v>1.04077</v>
+      </c>
+      <c r="AO23">
+        <v>1.0398700000000001</v>
+      </c>
+      <c r="AP23">
+        <v>1.0393300000000001</v>
+      </c>
+      <c r="AQ23">
+        <v>1.0458000000000001</v>
+      </c>
+      <c r="AR23">
+        <v>1.05026</v>
+      </c>
+      <c r="AS23">
+        <v>1.0684199999999999</v>
+      </c>
+      <c r="AT23">
+        <v>1.0855900000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2">
+        <f t="shared" si="0"/>
+        <v>2043</v>
+      </c>
+      <c r="C24" s="3">
+        <v>18890.3</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2.65</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.7588600000000001</v>
+      </c>
+      <c r="F24">
+        <v>53.734099999999998</v>
+      </c>
+      <c r="G24">
+        <v>335.47899999999998</v>
+      </c>
+      <c r="H24">
+        <v>483.209</v>
+      </c>
+      <c r="I24">
+        <v>367.76299999999998</v>
+      </c>
+      <c r="J24">
+        <v>252.87</v>
+      </c>
+      <c r="K24">
+        <v>263.05</v>
+      </c>
+      <c r="L24">
+        <v>729.23</v>
+      </c>
+      <c r="M24">
+        <v>8.73</v>
+      </c>
+      <c r="N24">
+        <v>10.39</v>
+      </c>
+      <c r="O24">
+        <v>2.39</v>
+      </c>
+      <c r="P24">
+        <v>5.6</v>
+      </c>
+      <c r="Q24" s="14">
+        <v>1.9247359164314057</v>
+      </c>
+      <c r="R24" s="14">
+        <v>7.3608773105891556</v>
+      </c>
+      <c r="S24" s="14">
+        <v>6.6399413510475673</v>
+      </c>
+      <c r="T24" s="2">
+        <v>2014.33</v>
+      </c>
+      <c r="U24" s="2">
+        <v>4119.3999999999996</v>
+      </c>
+      <c r="V24" s="2">
+        <v>10548.37</v>
+      </c>
+      <c r="W24" s="2">
+        <v>1</v>
+      </c>
+      <c r="X24" s="15">
+        <v>2064.6499000000003</v>
+      </c>
+      <c r="Y24" s="15">
+        <v>1.0151678765519685</v>
+      </c>
+      <c r="Z24" s="15">
+        <v>12677.771999999999</v>
+      </c>
+      <c r="AA24">
+        <v>1.11141</v>
+      </c>
+      <c r="AB24">
+        <v>1.1134900000000001</v>
+      </c>
+      <c r="AC24">
+        <v>1.1141700000000001</v>
+      </c>
+      <c r="AD24">
+        <v>1.11561</v>
+      </c>
+      <c r="AE24">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="AF24">
+        <v>1.11127</v>
+      </c>
+      <c r="AG24">
+        <v>1.1102399999999999</v>
+      </c>
+      <c r="AH24">
+        <v>1.1129100000000001</v>
+      </c>
+      <c r="AI24">
+        <v>1.1113900000000001</v>
+      </c>
+      <c r="AJ24">
+        <v>1.1172299999999999</v>
+      </c>
+      <c r="AK24">
+        <v>0.9839</v>
+      </c>
+      <c r="AL24">
+        <v>0.98902999999999996</v>
+      </c>
+      <c r="AM24">
+        <v>0.99791399999999997</v>
+      </c>
+      <c r="AN24">
+        <v>1.01014</v>
+      </c>
+      <c r="AO24">
+        <v>1.0092000000000001</v>
+      </c>
+      <c r="AP24">
+        <v>1.00865</v>
+      </c>
+      <c r="AQ24">
+        <v>1.01532</v>
+      </c>
+      <c r="AR24">
+        <v>1.01993</v>
+      </c>
+      <c r="AS24">
+        <v>1.0386599999999999</v>
+      </c>
+      <c r="AT24">
+        <v>1.0563800000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2">
+        <f t="shared" si="0"/>
+        <v>2044</v>
+      </c>
+      <c r="C25" s="3">
+        <v>19583.3</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2.64</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1.7477400000000001</v>
+      </c>
+      <c r="F25">
+        <v>53.802999999999997</v>
+      </c>
+      <c r="G25">
+        <v>335.91800000000001</v>
+      </c>
+      <c r="H25">
+        <v>483.54599999999999</v>
+      </c>
+      <c r="I25">
+        <v>367.85899999999998</v>
+      </c>
+      <c r="J25">
+        <v>253.32</v>
+      </c>
+      <c r="K25">
+        <v>262.48</v>
+      </c>
+      <c r="L25">
+        <v>730.36</v>
+      </c>
+      <c r="M25">
+        <v>9.07</v>
+      </c>
+      <c r="N25">
+        <v>10.79</v>
+      </c>
+      <c r="O25">
+        <v>2.48</v>
+      </c>
+      <c r="P25">
+        <v>5.78</v>
+      </c>
+      <c r="Q25" s="14">
+        <v>1.9942773110593004</v>
+      </c>
+      <c r="R25" s="14">
+        <v>7.6054908030514348</v>
+      </c>
+      <c r="S25" s="14">
+        <v>6.8915718451503061</v>
+      </c>
+      <c r="T25" s="2">
+        <v>2090.13</v>
+      </c>
+      <c r="U25" s="2">
+        <v>4245.5600000000004</v>
+      </c>
+      <c r="V25" s="2">
+        <v>10962.39</v>
+      </c>
+      <c r="W25" s="2">
+        <v>1</v>
+      </c>
+      <c r="X25" s="15">
+        <v>2147.9684000000002</v>
+      </c>
+      <c r="Y25" s="15">
+        <v>1.016060228865165</v>
+      </c>
+      <c r="Z25" s="15">
+        <v>13156.786</v>
+      </c>
+      <c r="AA25">
+        <v>1.1231500000000001</v>
+      </c>
+      <c r="AB25">
+        <v>1.1248</v>
+      </c>
+      <c r="AC25">
+        <v>1.12538</v>
+      </c>
+      <c r="AD25">
+        <v>1.12738</v>
+      </c>
+      <c r="AE25">
+        <v>1.12121</v>
+      </c>
+      <c r="AF25">
+        <v>1.12286</v>
+      </c>
+      <c r="AG25">
+        <v>1.12148</v>
+      </c>
+      <c r="AH25">
+        <v>1.12439</v>
+      </c>
+      <c r="AI25">
+        <v>1.1227100000000001</v>
+      </c>
+      <c r="AJ25">
+        <v>1.12927</v>
+      </c>
+      <c r="AK25">
+        <v>0.95260500000000004</v>
+      </c>
+      <c r="AL25">
+        <v>0.95794000000000001</v>
+      </c>
+      <c r="AM25">
+        <v>0.96717799999999998</v>
+      </c>
+      <c r="AN25">
+        <v>0.97989099999999996</v>
+      </c>
+      <c r="AO25">
+        <v>0.97892000000000001</v>
+      </c>
+      <c r="AP25">
+        <v>0.97834399999999999</v>
+      </c>
+      <c r="AQ25">
+        <v>0.98528499999999997</v>
+      </c>
+      <c r="AR25">
+        <v>0.99007400000000001</v>
+      </c>
+      <c r="AS25">
+        <v>1.00956</v>
+      </c>
+      <c r="AT25">
+        <v>1.0279799999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2">
+        <f t="shared" si="0"/>
+        <v>2045</v>
+      </c>
+      <c r="C26" s="3">
+        <v>20325.599999999999</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2.63</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1.7340599999999999</v>
+      </c>
+      <c r="F26">
+        <v>53.829599999999999</v>
+      </c>
+      <c r="G26">
+        <v>336.09399999999999</v>
+      </c>
+      <c r="H26">
+        <v>483.37400000000002</v>
+      </c>
+      <c r="I26">
+        <v>367.63900000000001</v>
+      </c>
+      <c r="J26">
+        <v>253.5</v>
+      </c>
+      <c r="K26">
+        <v>261.64</v>
+      </c>
+      <c r="L26">
+        <v>730.96</v>
+      </c>
+      <c r="M26">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="N26">
+        <v>11.25</v>
+      </c>
+      <c r="O26">
+        <v>2.57</v>
+      </c>
+      <c r="P26">
+        <v>5.99</v>
+      </c>
+      <c r="Q26" s="14">
+        <v>2.0713900610966225</v>
+      </c>
+      <c r="R26" s="14">
+        <v>7.8851327875129593</v>
+      </c>
+      <c r="S26" s="14">
+        <v>7.1791628686086222</v>
+      </c>
+      <c r="T26" s="2">
+        <v>2165.81</v>
+      </c>
+      <c r="U26" s="2">
+        <v>4382.71</v>
+      </c>
+      <c r="V26" s="2">
+        <v>11412.1</v>
+      </c>
+      <c r="W26" s="2">
+        <v>1</v>
+      </c>
+      <c r="X26" s="15">
+        <v>2232.5503999999996</v>
+      </c>
+      <c r="Y26" s="15">
+        <v>1.0160292901214811</v>
+      </c>
+      <c r="Z26" s="15">
+        <v>13670.663</v>
+      </c>
+      <c r="AA26">
+        <v>1.1249899999999999</v>
+      </c>
+      <c r="AB26">
+        <v>1.1265099999999999</v>
+      </c>
+      <c r="AC26">
+        <v>1.1270800000000001</v>
+      </c>
+      <c r="AD26">
+        <v>1.12931</v>
+      </c>
+      <c r="AE26">
+        <v>1.1229899999999999</v>
+      </c>
+      <c r="AF26">
+        <v>1.1248499999999999</v>
+      </c>
+      <c r="AG26">
+        <v>1.12331</v>
+      </c>
+      <c r="AH26">
+        <v>1.12626</v>
+      </c>
+      <c r="AI26">
+        <v>1.12459</v>
+      </c>
+      <c r="AJ26">
+        <v>1.13141</v>
+      </c>
+      <c r="AK26">
+        <v>0.93199900000000002</v>
+      </c>
+      <c r="AL26">
+        <v>0.93718000000000001</v>
+      </c>
+      <c r="AM26">
+        <v>0.94615099999999996</v>
+      </c>
+      <c r="AN26">
+        <v>0.95849600000000001</v>
+      </c>
+      <c r="AO26">
+        <v>0.95755299999999999</v>
+      </c>
+      <c r="AP26">
+        <v>0.95699299999999998</v>
+      </c>
+      <c r="AQ26">
+        <v>0.96373299999999995</v>
+      </c>
+      <c r="AR26">
+        <v>0.96838400000000002</v>
+      </c>
+      <c r="AS26">
+        <v>0.98730399999999996</v>
+      </c>
+      <c r="AT26">
+        <v>1.00519</v>
+      </c>
+    </row>
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2">
+        <f t="shared" si="0"/>
+        <v>2046</v>
+      </c>
+      <c r="C27" s="3">
+        <v>21129.7</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2.62</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1.7183999999999999</v>
+      </c>
+      <c r="F27">
+        <v>53.8185</v>
+      </c>
+      <c r="G27">
+        <v>335.98</v>
+      </c>
+      <c r="H27">
+        <v>482.49700000000001</v>
+      </c>
+      <c r="I27">
+        <v>367.19299999999998</v>
+      </c>
+      <c r="J27">
+        <v>252.17999999999998</v>
+      </c>
+      <c r="K27">
+        <v>261.01</v>
+      </c>
+      <c r="L27">
+        <v>731.47</v>
+      </c>
+      <c r="M27">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="N27">
+        <v>11.75</v>
+      </c>
+      <c r="O27">
+        <v>2.67</v>
+      </c>
+      <c r="P27">
+        <v>6.23</v>
+      </c>
+      <c r="Q27" s="14">
+        <v>2.1442334437932353</v>
+      </c>
+      <c r="R27" s="14">
+        <v>8.1898673381838165</v>
+      </c>
+      <c r="S27" s="14">
+        <v>7.4901140324200508</v>
+      </c>
+      <c r="T27" s="2">
+        <v>2240.23</v>
+      </c>
+      <c r="U27" s="2">
+        <v>4533.6400000000003</v>
+      </c>
+      <c r="V27" s="2">
+        <v>11902.11</v>
+      </c>
+      <c r="W27" s="2">
+        <v>1</v>
+      </c>
+      <c r="X27" s="15">
+        <v>2318.6769999999997</v>
+      </c>
+      <c r="Y27" s="15">
+        <v>1.0152206980339722</v>
+      </c>
+      <c r="Z27" s="15">
+        <v>14219.179</v>
+      </c>
+      <c r="AA27">
+        <v>1.1196299999999999</v>
+      </c>
+      <c r="AB27">
+        <v>1.1213299999999999</v>
+      </c>
+      <c r="AC27">
+        <v>1.12195</v>
+      </c>
+      <c r="AD27">
+        <v>1.1239600000000001</v>
+      </c>
+      <c r="AE27">
+        <v>1.1178300000000001</v>
+      </c>
+      <c r="AF27">
+        <v>1.1195900000000001</v>
+      </c>
+      <c r="AG27">
+        <v>1.11815</v>
+      </c>
+      <c r="AH27">
+        <v>1.1209899999999999</v>
+      </c>
+      <c r="AI27">
+        <v>1.11938</v>
+      </c>
+      <c r="AJ27">
+        <v>1.1259300000000001</v>
+      </c>
+      <c r="AK27">
+        <v>0.91520500000000005</v>
+      </c>
+      <c r="AL27">
+        <v>0.92000499999999996</v>
+      </c>
+      <c r="AM27">
+        <v>0.928315</v>
+      </c>
+      <c r="AN27">
+        <v>0.93975200000000003</v>
+      </c>
+      <c r="AO27">
+        <v>0.93887799999999999</v>
+      </c>
+      <c r="AP27">
+        <v>0.93835999999999997</v>
+      </c>
+      <c r="AQ27">
+        <v>0.944604</v>
+      </c>
+      <c r="AR27">
+        <v>0.94891199999999998</v>
+      </c>
+      <c r="AS27">
+        <v>0.96643900000000005</v>
+      </c>
+      <c r="AT27">
+        <v>0.98301000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2">
+        <f t="shared" si="0"/>
+        <v>2047</v>
+      </c>
+      <c r="C28" s="3">
+        <v>21914.7</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2.61</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1.7019200000000001</v>
+      </c>
+      <c r="F28">
+        <v>53.755899999999997</v>
+      </c>
+      <c r="G28">
+        <v>335.60700000000003</v>
+      </c>
+      <c r="H28">
+        <v>481.42200000000003</v>
+      </c>
+      <c r="I28">
+        <v>366.40899999999999</v>
+      </c>
+      <c r="J28">
+        <v>251.52</v>
+      </c>
+      <c r="K28">
+        <v>259.92</v>
+      </c>
+      <c r="L28">
+        <v>731.04</v>
+      </c>
+      <c r="M28">
+        <v>10.3</v>
+      </c>
+      <c r="N28">
+        <v>12.26</v>
+      </c>
+      <c r="O28">
+        <v>2.77</v>
+      </c>
+      <c r="P28">
+        <v>6.46</v>
+      </c>
+      <c r="Q28" s="14">
+        <v>2.2243298449561633</v>
+      </c>
+      <c r="R28" s="14">
+        <v>8.4979050384816261</v>
+      </c>
+      <c r="S28" s="14">
+        <v>7.8062320422443277</v>
+      </c>
+      <c r="T28" s="2">
+        <v>2318.2600000000002</v>
+      </c>
+      <c r="U28" s="2">
+        <v>4677.24</v>
+      </c>
+      <c r="V28" s="2">
+        <v>12377.02</v>
+      </c>
+      <c r="W28" s="2">
+        <v>1</v>
+      </c>
+      <c r="X28" s="15">
+        <v>2407.0526</v>
+      </c>
+      <c r="Y28" s="15">
+        <v>1.0149036891632148</v>
+      </c>
+      <c r="Z28" s="15">
+        <v>14760.723999999998</v>
+      </c>
+      <c r="AA28">
+        <v>1.12008</v>
+      </c>
+      <c r="AB28">
+        <v>1.12175</v>
+      </c>
+      <c r="AC28">
+        <v>1.1223799999999999</v>
+      </c>
+      <c r="AD28">
+        <v>1.1245700000000001</v>
+      </c>
+      <c r="AE28">
+        <v>1.1183399999999999</v>
+      </c>
+      <c r="AF28">
+        <v>1.1203000000000001</v>
+      </c>
+      <c r="AG28">
+        <v>1.11873</v>
+      </c>
+      <c r="AH28">
+        <v>1.12158</v>
+      </c>
+      <c r="AI28">
+        <v>1.12002</v>
+      </c>
+      <c r="AJ28">
+        <v>1.12677</v>
+      </c>
+      <c r="AK28">
+        <v>0.89843300000000004</v>
+      </c>
+      <c r="AL28">
+        <v>0.90289299999999995</v>
+      </c>
+      <c r="AM28">
+        <v>0.91061599999999998</v>
+      </c>
+      <c r="AN28">
+        <v>0.92124300000000003</v>
+      </c>
+      <c r="AO28">
+        <v>0.920431</v>
+      </c>
+      <c r="AP28">
+        <v>0.91994900000000002</v>
+      </c>
+      <c r="AQ28">
+        <v>0.92575099999999999</v>
+      </c>
+      <c r="AR28">
+        <v>0.929755</v>
+      </c>
+      <c r="AS28">
+        <v>0.94604100000000002</v>
+      </c>
+      <c r="AT28">
+        <v>0.96143900000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="C29" s="3">
+        <v>22719.7</v>
+      </c>
+      <c r="D29" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1.6829499999999999</v>
+      </c>
+      <c r="F29">
+        <v>53.640599999999999</v>
+      </c>
+      <c r="G29">
+        <v>334.54399999999998</v>
+      </c>
+      <c r="H29">
+        <v>479.94400000000002</v>
+      </c>
+      <c r="I29">
+        <v>365.065</v>
+      </c>
+      <c r="J29">
+        <v>250.67999999999998</v>
+      </c>
+      <c r="K29">
+        <v>258.76</v>
+      </c>
+      <c r="L29">
+        <v>728.83000000000015</v>
+      </c>
+      <c r="M29">
+        <v>10.76</v>
+      </c>
+      <c r="N29">
+        <v>12.75</v>
+      </c>
+      <c r="O29">
+        <v>2.88</v>
+      </c>
+      <c r="P29">
+        <v>6.71</v>
+      </c>
+      <c r="Q29" s="14">
+        <v>2.3137565693295148</v>
+      </c>
+      <c r="R29" s="14">
+        <v>8.8285118816869641</v>
+      </c>
+      <c r="S29" s="14">
+        <v>8.1155447146381938</v>
+      </c>
+      <c r="T29" s="2">
+        <v>2396.5300000000002</v>
+      </c>
+      <c r="U29" s="2">
+        <v>4829.8</v>
+      </c>
+      <c r="V29" s="2">
+        <v>12837.52</v>
+      </c>
+      <c r="W29" s="2">
+        <v>1</v>
+      </c>
+      <c r="X29" s="15">
+        <v>2496.1957000000002</v>
+      </c>
+      <c r="Y29" s="15">
+        <v>1.0135322843203416</v>
+      </c>
+      <c r="Z29" s="15">
+        <v>15297.189</v>
+      </c>
+      <c r="AA29">
+        <v>1.1157900000000001</v>
+      </c>
+      <c r="AB29">
+        <v>1.11765</v>
+      </c>
+      <c r="AC29">
+        <v>1.11833</v>
+      </c>
+      <c r="AD29">
+        <v>1.12039</v>
+      </c>
+      <c r="AE29">
+        <v>1.11429</v>
+      </c>
+      <c r="AF29">
+        <v>1.11622</v>
+      </c>
+      <c r="AG29">
+        <v>1.11469</v>
+      </c>
+      <c r="AH29">
+        <v>1.11747</v>
+      </c>
+      <c r="AI29">
+        <v>1.11599</v>
+      </c>
+      <c r="AJ29">
+        <v>1.12259</v>
+      </c>
+      <c r="AK29">
+        <v>0.88244100000000003</v>
+      </c>
+      <c r="AL29">
+        <v>0.88658599999999999</v>
+      </c>
+      <c r="AM29">
+        <v>0.89376199999999995</v>
+      </c>
+      <c r="AN29">
+        <v>0.90363700000000002</v>
+      </c>
+      <c r="AO29">
+        <v>0.90288299999999999</v>
+      </c>
+      <c r="AP29">
+        <v>0.90243499999999999</v>
+      </c>
+      <c r="AQ29">
+        <v>0.90782700000000005</v>
+      </c>
+      <c r="AR29">
+        <v>0.911547</v>
+      </c>
+      <c r="AS29">
+        <v>0.92668200000000001</v>
+      </c>
+      <c r="AT29">
+        <v>0.94098999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2">
+        <f t="shared" si="0"/>
+        <v>2049</v>
+      </c>
+      <c r="C30" s="3">
+        <v>23547.4</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2.59</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1.66022</v>
+      </c>
+      <c r="F30">
+        <v>53.429000000000002</v>
+      </c>
+      <c r="G30">
+        <v>333.00700000000001</v>
+      </c>
+      <c r="H30">
+        <v>477.31099999999998</v>
+      </c>
+      <c r="I30">
+        <v>363.04399999999998</v>
+      </c>
+      <c r="J30">
+        <v>248.92</v>
+      </c>
+      <c r="K30">
+        <v>257.05</v>
+      </c>
+      <c r="L30">
+        <v>725.85</v>
+      </c>
+      <c r="M30">
+        <v>11.28</v>
+      </c>
+      <c r="N30">
+        <v>13.32</v>
+      </c>
+      <c r="O30">
+        <v>2.99</v>
+      </c>
+      <c r="P30">
+        <v>6.98</v>
+      </c>
+      <c r="Q30" s="14">
+        <v>2.4050957918306342</v>
+      </c>
+      <c r="R30" s="14">
+        <v>9.1899784894488423</v>
+      </c>
+      <c r="S30" s="14">
+        <v>8.4709454067246099</v>
+      </c>
+      <c r="T30" s="2">
+        <v>2468.27</v>
+      </c>
+      <c r="U30" s="2">
+        <v>4980.37</v>
+      </c>
+      <c r="V30" s="2">
+        <v>13326.86</v>
+      </c>
+      <c r="W30" s="2">
+        <v>1</v>
+      </c>
+      <c r="X30" s="15">
+        <v>2584.855</v>
+      </c>
+      <c r="Y30" s="15">
+        <v>1.0118053476632585</v>
+      </c>
+      <c r="Z30" s="15">
+        <v>15848.884999999998</v>
+      </c>
+      <c r="AA30">
+        <v>1.1101799999999999</v>
+      </c>
+      <c r="AB30">
+        <v>1.1118399999999999</v>
+      </c>
+      <c r="AC30">
+        <v>1.1125</v>
+      </c>
+      <c r="AD30">
+        <v>1.1146499999999999</v>
+      </c>
+      <c r="AE30">
+        <v>1.10869</v>
+      </c>
+      <c r="AF30">
+        <v>1.11077</v>
+      </c>
+      <c r="AG30">
+        <v>1.10914</v>
+      </c>
+      <c r="AH30">
+        <v>1.11181</v>
+      </c>
+      <c r="AI30">
+        <v>1.11042</v>
+      </c>
+      <c r="AJ30">
+        <v>1.1169800000000001</v>
+      </c>
+      <c r="AK30">
+        <v>0.86766399999999999</v>
+      </c>
+      <c r="AL30">
+        <v>0.87150799999999995</v>
+      </c>
+      <c r="AM30">
+        <v>0.87816399999999994</v>
+      </c>
+      <c r="AN30">
+        <v>0.887324</v>
+      </c>
+      <c r="AO30">
+        <v>0.88662399999999997</v>
+      </c>
+      <c r="AP30">
+        <v>0.88620900000000002</v>
+      </c>
+      <c r="AQ30">
+        <v>0.89120999999999995</v>
+      </c>
+      <c r="AR30">
+        <v>0.89466100000000004</v>
+      </c>
+      <c r="AS30">
+        <v>0.90869900000000003</v>
+      </c>
+      <c r="AT30">
+        <v>0.92197099999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+      <c r="C31" s="3">
+        <v>24294</v>
+      </c>
+      <c r="D31" s="3">
+        <v>2.57</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1.6348499999999999</v>
+      </c>
+      <c r="F31">
+        <v>53.110999999999997</v>
+      </c>
+      <c r="G31">
+        <v>330.94</v>
+      </c>
+      <c r="H31">
+        <v>474.13499999999999</v>
+      </c>
+      <c r="I31">
+        <v>360.178</v>
+      </c>
+      <c r="J31">
+        <v>248.8</v>
+      </c>
+      <c r="K31">
+        <v>254.15</v>
+      </c>
+      <c r="L31">
+        <v>720.82999999999993</v>
+      </c>
+      <c r="M31">
+        <v>11.82</v>
+      </c>
+      <c r="N31">
+        <v>13.94</v>
+      </c>
+      <c r="O31">
+        <v>3.12</v>
+      </c>
+      <c r="P31">
+        <v>7.25</v>
+      </c>
+      <c r="Q31" s="14">
+        <v>2.519197719171447</v>
+      </c>
+      <c r="R31" s="14">
+        <v>9.5693572620297651</v>
+      </c>
+      <c r="S31" s="14">
+        <v>8.8553862444508553</v>
+      </c>
+      <c r="T31" s="2">
+        <v>2549.54</v>
+      </c>
+      <c r="U31" s="2">
+        <v>5108.8100000000004</v>
+      </c>
+      <c r="V31" s="2">
+        <v>13774.1</v>
+      </c>
+      <c r="W31" s="2">
+        <v>1</v>
+      </c>
+      <c r="X31" s="15">
+        <v>2673.8330000000005</v>
+      </c>
+      <c r="Y31" s="15">
+        <v>1.0118717242401116</v>
+      </c>
+      <c r="Z31" s="15">
+        <v>16377.313000000002</v>
+      </c>
+      <c r="AA31">
+        <v>1.1170899999999999</v>
+      </c>
+      <c r="AB31">
+        <v>1.11846</v>
+      </c>
+      <c r="AC31">
+        <v>1.1190599999999999</v>
+      </c>
+      <c r="AD31">
+        <v>1.1215599999999999</v>
+      </c>
+      <c r="AE31">
+        <v>1.11528</v>
+      </c>
+      <c r="AF31">
+        <v>1.1176200000000001</v>
+      </c>
+      <c r="AG31">
+        <v>1.11574</v>
+      </c>
+      <c r="AH31">
+        <v>1.11853</v>
+      </c>
+      <c r="AI31">
+        <v>1.1170500000000001</v>
+      </c>
+      <c r="AJ31">
+        <v>1.12395</v>
+      </c>
+      <c r="AK31">
+        <v>0.85139799999999999</v>
+      </c>
+      <c r="AL31">
+        <v>0.85505299999999995</v>
+      </c>
+      <c r="AM31">
+        <v>0.86138300000000001</v>
+      </c>
+      <c r="AN31">
+        <v>0.87009400000000003</v>
+      </c>
+      <c r="AO31">
+        <v>0.86942900000000001</v>
+      </c>
+      <c r="AP31">
+        <v>0.86903399999999997</v>
+      </c>
+      <c r="AQ31">
+        <v>0.87378999999999996</v>
+      </c>
+      <c r="AR31">
+        <v>0.87707199999999996</v>
+      </c>
+      <c r="AS31">
+        <v>0.89042100000000002</v>
+      </c>
+      <c r="AT31">
+        <v>0.90304300000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="2"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="15"/>
+      <c r="Y32" s="15"/>
+      <c r="Z32" s="15"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="2"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="15"/>
+      <c r="Y33" s="15"/>
+      <c r="Z33" s="15"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="2"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="15"/>
+      <c r="Y34" s="15"/>
+      <c r="Z34" s="15"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="2"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="15"/>
+      <c r="Y35" s="15"/>
+      <c r="Z35" s="15"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="2"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="15"/>
+      <c r="Y36" s="15"/>
+      <c r="Z36" s="15"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="2"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="15"/>
+      <c r="Y37" s="15"/>
+      <c r="Z37" s="15"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="2"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="15"/>
+      <c r="Y38" s="15"/>
+      <c r="Z38" s="15"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="2"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="15"/>
+      <c r="Y39" s="15"/>
+      <c r="Z39" s="15"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="2"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="15"/>
+      <c r="Y40" s="15"/>
+      <c r="Z40" s="15"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="2"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="15"/>
+      <c r="Y41" s="15"/>
+      <c r="Z41" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="AK1:AT1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="AA1:AJ1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added back carbon tax revenues
</commit_message>
<xml_diff>
--- a/data/ARM-Microsimulation/ARM_MacroScenarioInformation.xlsx
+++ b/data/ARM-Microsimulation/ARM_MacroScenarioInformation.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\armenia-ccdr\data\ARM-Microsimulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62679D45-80CF-4462-9FF0-061DDFD9619E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF5D747-5AEF-411A-A9A1-F42341C2DB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{66FC96EB-762B-4856-BAC6-F6820D271721}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{66FC96EB-762B-4856-BAC6-F6820D271721}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="8" r:id="rId1"/>
     <sheet name="Dry-hot scenario" sheetId="9" r:id="rId2"/>
-    <sheet name="NZS" sheetId="10" r:id="rId3"/>
+    <sheet name="NZS" sheetId="11" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -141,12 +141,19 @@
   <si>
     <t>Energy (gas, oil, coal, electricity) price index</t>
   </si>
+  <si>
+    <t>Government transfers of carbon tax revenue (billion AMD)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +171,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -324,10 +338,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -410,9 +425,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -10808,11 +10832,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7085DB3-4548-46EC-8A84-75E007D14A48}">
-  <dimension ref="A1:AT41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB83E350-2124-45AA-B8F7-7F424DD6AEA3}">
+  <dimension ref="A1:BD170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10825,7 +10849,7 @@
     <col min="26" max="26" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -10886,8 +10910,20 @@
       <c r="AR1" s="26"/>
       <c r="AS1" s="26"/>
       <c r="AT1" s="27"/>
-    </row>
-    <row r="2" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+      <c r="AU1" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="AV1" s="33"/>
+      <c r="AW1" s="33"/>
+      <c r="AX1" s="33"/>
+      <c r="AY1" s="33"/>
+      <c r="AZ1" s="33"/>
+      <c r="BA1" s="33"/>
+      <c r="BB1" s="33"/>
+      <c r="BC1" s="33"/>
+      <c r="BD1" s="33"/>
+    </row>
+    <row r="2" spans="1:56" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -11026,8 +11062,38 @@
       <c r="AT2" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AW2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AY2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AZ2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="BA2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="BB2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="BC2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="BD2" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>45455</v>
       </c>
@@ -11167,7 +11233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2">
         <f>B3+1</f>
@@ -11305,8 +11371,38 @@
       <c r="AT4">
         <v>1.2590699999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU4">
+        <v>3.8545581388500003</v>
+      </c>
+      <c r="AV4">
+        <v>3.8545581388500003</v>
+      </c>
+      <c r="AW4">
+        <v>3.8545581388500003</v>
+      </c>
+      <c r="AX4">
+        <v>3.8545581388500003</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4">
+        <v>0</v>
+      </c>
+      <c r="BA4">
+        <v>0</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+      <c r="BC4">
+        <v>0</v>
+      </c>
+      <c r="BD4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2">
         <f t="shared" ref="B5:B40" si="0">B4+1</f>
@@ -11444,8 +11540,38 @@
       <c r="AT5">
         <v>1.4189700000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU5">
+        <v>7.0566295770000007</v>
+      </c>
+      <c r="AV5">
+        <v>7.0566295770000007</v>
+      </c>
+      <c r="AW5">
+        <v>7.0566295770000007</v>
+      </c>
+      <c r="AX5">
+        <v>7.0566295770000007</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="AZ5">
+        <v>0</v>
+      </c>
+      <c r="BA5">
+        <v>0</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
+      <c r="BC5">
+        <v>0</v>
+      </c>
+      <c r="BD5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2">
         <f t="shared" si="0"/>
@@ -11583,8 +11709,38 @@
       <c r="AT6">
         <v>1.58616</v>
       </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU6">
+        <v>10.222593444000001</v>
+      </c>
+      <c r="AV6">
+        <v>10.222593444000001</v>
+      </c>
+      <c r="AW6">
+        <v>10.222593444000001</v>
+      </c>
+      <c r="AX6">
+        <v>10.222593444000001</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
+      </c>
+      <c r="AZ6">
+        <v>0</v>
+      </c>
+      <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6">
+        <v>0</v>
+      </c>
+      <c r="BC6">
+        <v>0</v>
+      </c>
+      <c r="BD6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2">
         <f t="shared" si="0"/>
@@ -11722,8 +11878,38 @@
       <c r="AT7">
         <v>1.72712</v>
       </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU7">
+        <v>13.288198284</v>
+      </c>
+      <c r="AV7">
+        <v>13.288198284</v>
+      </c>
+      <c r="AW7">
+        <v>13.288198284</v>
+      </c>
+      <c r="AX7">
+        <v>13.288198284</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
+      </c>
+      <c r="AZ7">
+        <v>0</v>
+      </c>
+      <c r="BA7">
+        <v>0</v>
+      </c>
+      <c r="BB7">
+        <v>0</v>
+      </c>
+      <c r="BC7">
+        <v>0</v>
+      </c>
+      <c r="BD7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2">
         <f t="shared" si="0"/>
@@ -11861,8 +12047,38 @@
       <c r="AT8">
         <v>1.8523799999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU8">
+        <v>16.316885794499999</v>
+      </c>
+      <c r="AV8">
+        <v>16.316885794499999</v>
+      </c>
+      <c r="AW8">
+        <v>16.316885794499999</v>
+      </c>
+      <c r="AX8">
+        <v>16.316885794499999</v>
+      </c>
+      <c r="AY8">
+        <v>0</v>
+      </c>
+      <c r="AZ8">
+        <v>0</v>
+      </c>
+      <c r="BA8">
+        <v>0</v>
+      </c>
+      <c r="BB8">
+        <v>0</v>
+      </c>
+      <c r="BC8">
+        <v>0</v>
+      </c>
+      <c r="BD8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2">
         <f t="shared" si="0"/>
@@ -12000,8 +12216,38 @@
       <c r="AT9">
         <v>1.96347</v>
       </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU9">
+        <v>19.309931185500002</v>
+      </c>
+      <c r="AV9">
+        <v>19.309931185500002</v>
+      </c>
+      <c r="AW9">
+        <v>19.309931185500002</v>
+      </c>
+      <c r="AX9">
+        <v>19.309931185500002</v>
+      </c>
+      <c r="AY9">
+        <v>0</v>
+      </c>
+      <c r="AZ9">
+        <v>0</v>
+      </c>
+      <c r="BA9">
+        <v>0</v>
+      </c>
+      <c r="BB9">
+        <v>0</v>
+      </c>
+      <c r="BC9">
+        <v>0</v>
+      </c>
+      <c r="BD9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
@@ -12139,8 +12385,38 @@
       <c r="AT10">
         <v>2.0590799999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU10">
+        <v>22.266314289</v>
+      </c>
+      <c r="AV10">
+        <v>22.266314289</v>
+      </c>
+      <c r="AW10">
+        <v>22.266314289</v>
+      </c>
+      <c r="AX10">
+        <v>22.266314289</v>
+      </c>
+      <c r="AY10">
+        <v>0</v>
+      </c>
+      <c r="AZ10">
+        <v>0</v>
+      </c>
+      <c r="BA10">
+        <v>0</v>
+      </c>
+      <c r="BB10">
+        <v>0</v>
+      </c>
+      <c r="BC10">
+        <v>0</v>
+      </c>
+      <c r="BD10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
@@ -12278,8 +12554,38 @@
       <c r="AT11">
         <v>2.1307499999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU11">
+        <v>25.152050758500003</v>
+      </c>
+      <c r="AV11">
+        <v>25.152050758500003</v>
+      </c>
+      <c r="AW11">
+        <v>25.152050758500003</v>
+      </c>
+      <c r="AX11">
+        <v>25.152050758500003</v>
+      </c>
+      <c r="AY11">
+        <v>0</v>
+      </c>
+      <c r="AZ11">
+        <v>0</v>
+      </c>
+      <c r="BA11">
+        <v>0</v>
+      </c>
+      <c r="BB11">
+        <v>0</v>
+      </c>
+      <c r="BC11">
+        <v>0</v>
+      </c>
+      <c r="BD11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
@@ -12417,8 +12723,38 @@
       <c r="AT12">
         <v>2.1114099999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU12">
+        <v>26.337294693</v>
+      </c>
+      <c r="AV12">
+        <v>26.337294693</v>
+      </c>
+      <c r="AW12">
+        <v>26.337294693</v>
+      </c>
+      <c r="AX12">
+        <v>26.337294693</v>
+      </c>
+      <c r="AY12">
+        <v>0</v>
+      </c>
+      <c r="AZ12">
+        <v>0</v>
+      </c>
+      <c r="BA12">
+        <v>0</v>
+      </c>
+      <c r="BB12">
+        <v>0</v>
+      </c>
+      <c r="BC12">
+        <v>0</v>
+      </c>
+      <c r="BD12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2">
         <f t="shared" si="0"/>
@@ -12556,8 +12892,38 @@
       <c r="AT13">
         <v>2.0870799999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU13">
+        <v>27.448576447499999</v>
+      </c>
+      <c r="AV13">
+        <v>27.448576447499999</v>
+      </c>
+      <c r="AW13">
+        <v>27.448576447499999</v>
+      </c>
+      <c r="AX13">
+        <v>27.448576447499999</v>
+      </c>
+      <c r="AY13">
+        <v>0</v>
+      </c>
+      <c r="AZ13">
+        <v>0</v>
+      </c>
+      <c r="BA13">
+        <v>0</v>
+      </c>
+      <c r="BB13">
+        <v>0</v>
+      </c>
+      <c r="BC13">
+        <v>0</v>
+      </c>
+      <c r="BD13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
@@ -12695,8 +13061,38 @@
       <c r="AT14">
         <v>2.0661999999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU14">
+        <v>28.405430271000004</v>
+      </c>
+      <c r="AV14">
+        <v>28.405430271000004</v>
+      </c>
+      <c r="AW14">
+        <v>28.405430271000004</v>
+      </c>
+      <c r="AX14">
+        <v>28.405430271000004</v>
+      </c>
+      <c r="AY14">
+        <v>0</v>
+      </c>
+      <c r="AZ14">
+        <v>0</v>
+      </c>
+      <c r="BA14">
+        <v>0</v>
+      </c>
+      <c r="BB14">
+        <v>0</v>
+      </c>
+      <c r="BC14">
+        <v>0</v>
+      </c>
+      <c r="BD14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
@@ -12834,8 +13230,38 @@
       <c r="AT15">
         <v>2.04054</v>
       </c>
-    </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU15">
+        <v>29.266260781499998</v>
+      </c>
+      <c r="AV15">
+        <v>29.266260781499998</v>
+      </c>
+      <c r="AW15">
+        <v>29.266260781499998</v>
+      </c>
+      <c r="AX15">
+        <v>29.266260781499998</v>
+      </c>
+      <c r="AY15">
+        <v>0</v>
+      </c>
+      <c r="AZ15">
+        <v>0</v>
+      </c>
+      <c r="BA15">
+        <v>0</v>
+      </c>
+      <c r="BB15">
+        <v>0</v>
+      </c>
+      <c r="BC15">
+        <v>0</v>
+      </c>
+      <c r="BD15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
@@ -12973,8 +13399,38 @@
       <c r="AT16">
         <v>2.00787</v>
       </c>
-    </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU16">
+        <v>29.909349184500002</v>
+      </c>
+      <c r="AV16">
+        <v>29.909349184500002</v>
+      </c>
+      <c r="AW16">
+        <v>29.909349184500002</v>
+      </c>
+      <c r="AX16">
+        <v>29.909349184500002</v>
+      </c>
+      <c r="AY16">
+        <v>0</v>
+      </c>
+      <c r="AZ16">
+        <v>0</v>
+      </c>
+      <c r="BA16">
+        <v>0</v>
+      </c>
+      <c r="BB16">
+        <v>0</v>
+      </c>
+      <c r="BC16">
+        <v>0</v>
+      </c>
+      <c r="BD16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
@@ -13112,8 +13568,38 @@
       <c r="AT17">
         <v>1.8510200000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU17">
+        <v>29.946457795499999</v>
+      </c>
+      <c r="AV17">
+        <v>29.946457795499999</v>
+      </c>
+      <c r="AW17">
+        <v>29.946457795499999</v>
+      </c>
+      <c r="AX17">
+        <v>29.946457795499999</v>
+      </c>
+      <c r="AY17">
+        <v>0</v>
+      </c>
+      <c r="AZ17">
+        <v>0</v>
+      </c>
+      <c r="BA17">
+        <v>0</v>
+      </c>
+      <c r="BB17">
+        <v>0</v>
+      </c>
+      <c r="BC17">
+        <v>0</v>
+      </c>
+      <c r="BD17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2">
         <f t="shared" si="0"/>
@@ -13251,8 +13737,38 @@
       <c r="AT18">
         <v>1.7057800000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU18">
+        <v>29.874344669999999</v>
+      </c>
+      <c r="AV18">
+        <v>29.874344669999999</v>
+      </c>
+      <c r="AW18">
+        <v>29.874344669999999</v>
+      </c>
+      <c r="AX18">
+        <v>29.874344669999999</v>
+      </c>
+      <c r="AY18">
+        <v>0</v>
+      </c>
+      <c r="AZ18">
+        <v>0</v>
+      </c>
+      <c r="BA18">
+        <v>0</v>
+      </c>
+      <c r="BB18">
+        <v>0</v>
+      </c>
+      <c r="BC18">
+        <v>0</v>
+      </c>
+      <c r="BD18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2">
         <f t="shared" si="0"/>
@@ -13390,8 +13906,38 @@
       <c r="AT19">
         <v>1.5733900000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU19">
+        <v>29.6998321815</v>
+      </c>
+      <c r="AV19">
+        <v>29.6998321815</v>
+      </c>
+      <c r="AW19">
+        <v>29.6998321815</v>
+      </c>
+      <c r="AX19">
+        <v>29.6998321815</v>
+      </c>
+      <c r="AY19">
+        <v>0</v>
+      </c>
+      <c r="AZ19">
+        <v>0</v>
+      </c>
+      <c r="BA19">
+        <v>0</v>
+      </c>
+      <c r="BB19">
+        <v>0</v>
+      </c>
+      <c r="BC19">
+        <v>0</v>
+      </c>
+      <c r="BD19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2">
         <f t="shared" si="0"/>
@@ -13529,8 +14075,38 @@
       <c r="AT20">
         <v>1.45201</v>
       </c>
-    </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU20">
+        <v>29.435863711500001</v>
+      </c>
+      <c r="AV20">
+        <v>29.435863711500001</v>
+      </c>
+      <c r="AW20">
+        <v>29.435863711500001</v>
+      </c>
+      <c r="AX20">
+        <v>29.435863711500001</v>
+      </c>
+      <c r="AY20">
+        <v>0</v>
+      </c>
+      <c r="AZ20">
+        <v>0</v>
+      </c>
+      <c r="BA20">
+        <v>0</v>
+      </c>
+      <c r="BB20">
+        <v>0</v>
+      </c>
+      <c r="BC20">
+        <v>0</v>
+      </c>
+      <c r="BD20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2">
         <f t="shared" si="0"/>
@@ -13668,8 +14244,38 @@
       <c r="AT21">
         <v>1.3388199999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU21">
+        <v>29.091557011500001</v>
+      </c>
+      <c r="AV21">
+        <v>29.091557011500001</v>
+      </c>
+      <c r="AW21">
+        <v>29.091557011500001</v>
+      </c>
+      <c r="AX21">
+        <v>29.091557011500001</v>
+      </c>
+      <c r="AY21">
+        <v>0</v>
+      </c>
+      <c r="AZ21">
+        <v>0</v>
+      </c>
+      <c r="BA21">
+        <v>0</v>
+      </c>
+      <c r="BB21">
+        <v>0</v>
+      </c>
+      <c r="BC21">
+        <v>0</v>
+      </c>
+      <c r="BD21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2">
         <f t="shared" si="0"/>
@@ -13807,8 +14413,38 @@
       <c r="AT22">
         <v>1.21289</v>
       </c>
-    </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU22">
+        <v>28.492335832499997</v>
+      </c>
+      <c r="AV22">
+        <v>28.492335832499997</v>
+      </c>
+      <c r="AW22">
+        <v>28.492335832499997</v>
+      </c>
+      <c r="AX22">
+        <v>28.492335832499997</v>
+      </c>
+      <c r="AY22">
+        <v>0</v>
+      </c>
+      <c r="AZ22">
+        <v>0</v>
+      </c>
+      <c r="BA22">
+        <v>0</v>
+      </c>
+      <c r="BB22">
+        <v>0</v>
+      </c>
+      <c r="BC22">
+        <v>0</v>
+      </c>
+      <c r="BD22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2">
         <f t="shared" si="0"/>
@@ -13946,8 +14582,38 @@
       <c r="AT23">
         <v>1.0992</v>
       </c>
-    </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU23">
+        <v>27.831394489499999</v>
+      </c>
+      <c r="AV23">
+        <v>27.831394489499999</v>
+      </c>
+      <c r="AW23">
+        <v>27.831394489499999</v>
+      </c>
+      <c r="AX23">
+        <v>27.831394489499999</v>
+      </c>
+      <c r="AY23">
+        <v>0</v>
+      </c>
+      <c r="AZ23">
+        <v>0</v>
+      </c>
+      <c r="BA23">
+        <v>0</v>
+      </c>
+      <c r="BB23">
+        <v>0</v>
+      </c>
+      <c r="BC23">
+        <v>0</v>
+      </c>
+      <c r="BD23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2">
         <f t="shared" si="0"/>
@@ -14085,8 +14751,38 @@
       <c r="AT24">
         <v>0.99581900000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU24">
+        <v>27.127032246000002</v>
+      </c>
+      <c r="AV24">
+        <v>27.127032246000002</v>
+      </c>
+      <c r="AW24">
+        <v>27.127032246000002</v>
+      </c>
+      <c r="AX24">
+        <v>27.127032246000002</v>
+      </c>
+      <c r="AY24">
+        <v>0</v>
+      </c>
+      <c r="AZ24">
+        <v>0</v>
+      </c>
+      <c r="BA24">
+        <v>0</v>
+      </c>
+      <c r="BB24">
+        <v>0</v>
+      </c>
+      <c r="BC24">
+        <v>0</v>
+      </c>
+      <c r="BD24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2">
         <f t="shared" si="0"/>
@@ -14224,8 +14920,38 @@
       <c r="AT25">
         <v>0.90250900000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU25">
+        <v>26.393658975000001</v>
+      </c>
+      <c r="AV25">
+        <v>26.393658975000001</v>
+      </c>
+      <c r="AW25">
+        <v>26.393658975000001</v>
+      </c>
+      <c r="AX25">
+        <v>26.393658975000001</v>
+      </c>
+      <c r="AY25">
+        <v>0</v>
+      </c>
+      <c r="AZ25">
+        <v>0</v>
+      </c>
+      <c r="BA25">
+        <v>0</v>
+      </c>
+      <c r="BB25">
+        <v>0</v>
+      </c>
+      <c r="BC25">
+        <v>0</v>
+      </c>
+      <c r="BD25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2">
         <f t="shared" si="0"/>
@@ -14363,8 +15089,38 @@
       <c r="AT26">
         <v>0.82677599999999996</v>
       </c>
-    </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU26">
+        <v>25.637204403000002</v>
+      </c>
+      <c r="AV26">
+        <v>25.637204403000002</v>
+      </c>
+      <c r="AW26">
+        <v>25.637204403000002</v>
+      </c>
+      <c r="AX26">
+        <v>25.637204403000002</v>
+      </c>
+      <c r="AY26">
+        <v>0</v>
+      </c>
+      <c r="AZ26">
+        <v>0</v>
+      </c>
+      <c r="BA26">
+        <v>0</v>
+      </c>
+      <c r="BB26">
+        <v>0</v>
+      </c>
+      <c r="BC26">
+        <v>0</v>
+      </c>
+      <c r="BD26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2">
         <f t="shared" si="0"/>
@@ -14502,8 +15258,38 @@
       <c r="AT27">
         <v>0.78683000000000003</v>
       </c>
-    </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU27">
+        <v>25.246990143000001</v>
+      </c>
+      <c r="AV27">
+        <v>25.246990143000001</v>
+      </c>
+      <c r="AW27">
+        <v>25.246990143000001</v>
+      </c>
+      <c r="AX27">
+        <v>25.246990143000001</v>
+      </c>
+      <c r="AY27">
+        <v>0</v>
+      </c>
+      <c r="AZ27">
+        <v>0</v>
+      </c>
+      <c r="BA27">
+        <v>0</v>
+      </c>
+      <c r="BB27">
+        <v>0</v>
+      </c>
+      <c r="BC27">
+        <v>0</v>
+      </c>
+      <c r="BD27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2">
         <f t="shared" si="0"/>
@@ -14641,8 +15427,38 @@
       <c r="AT28">
         <v>0.75227200000000005</v>
       </c>
-    </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU28">
+        <v>24.830315275499999</v>
+      </c>
+      <c r="AV28">
+        <v>24.830315275499999</v>
+      </c>
+      <c r="AW28">
+        <v>24.830315275499999</v>
+      </c>
+      <c r="AX28">
+        <v>24.830315275499999</v>
+      </c>
+      <c r="AY28">
+        <v>0</v>
+      </c>
+      <c r="AZ28">
+        <v>0</v>
+      </c>
+      <c r="BA28">
+        <v>0</v>
+      </c>
+      <c r="BB28">
+        <v>0</v>
+      </c>
+      <c r="BC28">
+        <v>0</v>
+      </c>
+      <c r="BD28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2">
         <f t="shared" si="0"/>
@@ -14780,8 +15596,38 @@
       <c r="AT29">
         <v>0.72350999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU29">
+        <v>24.382078960500003</v>
+      </c>
+      <c r="AV29">
+        <v>24.382078960500003</v>
+      </c>
+      <c r="AW29">
+        <v>24.382078960500003</v>
+      </c>
+      <c r="AX29">
+        <v>24.382078960500003</v>
+      </c>
+      <c r="AY29">
+        <v>0</v>
+      </c>
+      <c r="AZ29">
+        <v>0</v>
+      </c>
+      <c r="BA29">
+        <v>0</v>
+      </c>
+      <c r="BB29">
+        <v>0</v>
+      </c>
+      <c r="BC29">
+        <v>0</v>
+      </c>
+      <c r="BD29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2">
         <f t="shared" si="0"/>
@@ -14919,8 +15765,38 @@
       <c r="AT30">
         <v>0.70027799999999996</v>
       </c>
-    </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU30">
+        <v>23.903173845000005</v>
+      </c>
+      <c r="AV30">
+        <v>23.903173845000005</v>
+      </c>
+      <c r="AW30">
+        <v>23.903173845000005</v>
+      </c>
+      <c r="AX30">
+        <v>23.903173845000005</v>
+      </c>
+      <c r="AY30">
+        <v>0</v>
+      </c>
+      <c r="AZ30">
+        <v>0</v>
+      </c>
+      <c r="BA30">
+        <v>0</v>
+      </c>
+      <c r="BB30">
+        <v>0</v>
+      </c>
+      <c r="BC30">
+        <v>0</v>
+      </c>
+      <c r="BD30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2">
         <f t="shared" si="0"/>
@@ -15058,8 +15934,38 @@
       <c r="AT31">
         <v>0.67012799999999995</v>
       </c>
-    </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU31">
+        <v>23.416362427500005</v>
+      </c>
+      <c r="AV31">
+        <v>23.416362427500005</v>
+      </c>
+      <c r="AW31">
+        <v>23.416362427500005</v>
+      </c>
+      <c r="AX31">
+        <v>23.416362427500005</v>
+      </c>
+      <c r="AY31">
+        <v>0</v>
+      </c>
+      <c r="AZ31">
+        <v>0</v>
+      </c>
+      <c r="BA31">
+        <v>0</v>
+      </c>
+      <c r="BB31">
+        <v>0</v>
+      </c>
+      <c r="BC31">
+        <v>0</v>
+      </c>
+      <c r="BD31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2">
         <f t="shared" si="0"/>
@@ -15197,8 +16103,38 @@
       <c r="AT32">
         <v>0.62656800000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU32">
+        <v>23.225654771999999</v>
+      </c>
+      <c r="AV32">
+        <v>23.225654771999999</v>
+      </c>
+      <c r="AW32">
+        <v>23.225654771999999</v>
+      </c>
+      <c r="AX32">
+        <v>23.225654771999999</v>
+      </c>
+      <c r="AY32">
+        <v>0</v>
+      </c>
+      <c r="AZ32">
+        <v>0</v>
+      </c>
+      <c r="BA32">
+        <v>0</v>
+      </c>
+      <c r="BB32">
+        <v>0</v>
+      </c>
+      <c r="BC32">
+        <v>0</v>
+      </c>
+      <c r="BD32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2">
         <f t="shared" si="0"/>
@@ -15336,8 +16272,38 @@
       <c r="AT33">
         <v>0.58693300000000004</v>
       </c>
-    </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU33">
+        <v>22.992418863000001</v>
+      </c>
+      <c r="AV33">
+        <v>22.992418863000001</v>
+      </c>
+      <c r="AW33">
+        <v>22.992418863000001</v>
+      </c>
+      <c r="AX33">
+        <v>22.992418863000001</v>
+      </c>
+      <c r="AY33">
+        <v>0</v>
+      </c>
+      <c r="AZ33">
+        <v>0</v>
+      </c>
+      <c r="BA33">
+        <v>0</v>
+      </c>
+      <c r="BB33">
+        <v>0</v>
+      </c>
+      <c r="BC33">
+        <v>0</v>
+      </c>
+      <c r="BD33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2">
         <f t="shared" si="0"/>
@@ -15475,8 +16441,38 @@
       <c r="AT34">
         <v>0.55064299999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU34">
+        <v>22.718758797000003</v>
+      </c>
+      <c r="AV34">
+        <v>22.718758797000003</v>
+      </c>
+      <c r="AW34">
+        <v>22.718758797000003</v>
+      </c>
+      <c r="AX34">
+        <v>22.718758797000003</v>
+      </c>
+      <c r="AY34">
+        <v>0</v>
+      </c>
+      <c r="AZ34">
+        <v>0</v>
+      </c>
+      <c r="BA34">
+        <v>0</v>
+      </c>
+      <c r="BB34">
+        <v>0</v>
+      </c>
+      <c r="BC34">
+        <v>0</v>
+      </c>
+      <c r="BD34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2">
         <f t="shared" si="0"/>
@@ -15614,8 +16610,38 @@
       <c r="AT35">
         <v>0.51763199999999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU35">
+        <v>22.366035711000002</v>
+      </c>
+      <c r="AV35">
+        <v>22.366035711000002</v>
+      </c>
+      <c r="AW35">
+        <v>22.366035711000002</v>
+      </c>
+      <c r="AX35">
+        <v>22.366035711000002</v>
+      </c>
+      <c r="AY35">
+        <v>0</v>
+      </c>
+      <c r="AZ35">
+        <v>0</v>
+      </c>
+      <c r="BA35">
+        <v>0</v>
+      </c>
+      <c r="BB35">
+        <v>0</v>
+      </c>
+      <c r="BC35">
+        <v>0</v>
+      </c>
+      <c r="BD35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2">
         <f t="shared" si="0"/>
@@ -15753,8 +16779,38 @@
       <c r="AT36">
         <v>0.50518099999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU36">
+        <v>21.943558637999999</v>
+      </c>
+      <c r="AV36">
+        <v>21.943558637999999</v>
+      </c>
+      <c r="AW36">
+        <v>21.943558637999999</v>
+      </c>
+      <c r="AX36">
+        <v>21.943558637999999</v>
+      </c>
+      <c r="AY36">
+        <v>0</v>
+      </c>
+      <c r="AZ36">
+        <v>0</v>
+      </c>
+      <c r="BA36">
+        <v>0</v>
+      </c>
+      <c r="BB36">
+        <v>0</v>
+      </c>
+      <c r="BC36">
+        <v>0</v>
+      </c>
+      <c r="BD36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2">
         <f t="shared" si="0"/>
@@ -15892,8 +16948,38 @@
       <c r="AT37">
         <v>0.49613000000000002</v>
       </c>
-    </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU37">
+        <v>21.753042264000001</v>
+      </c>
+      <c r="AV37">
+        <v>21.753042264000001</v>
+      </c>
+      <c r="AW37">
+        <v>21.753042264000001</v>
+      </c>
+      <c r="AX37">
+        <v>21.753042264000001</v>
+      </c>
+      <c r="AY37">
+        <v>0</v>
+      </c>
+      <c r="AZ37">
+        <v>0</v>
+      </c>
+      <c r="BA37">
+        <v>0</v>
+      </c>
+      <c r="BB37">
+        <v>0</v>
+      </c>
+      <c r="BC37">
+        <v>0</v>
+      </c>
+      <c r="BD37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2">
         <f t="shared" si="0"/>
@@ -16031,8 +17117,38 @@
       <c r="AT38">
         <v>0.48925800000000003</v>
       </c>
-    </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU38">
+        <v>21.516682090500002</v>
+      </c>
+      <c r="AV38">
+        <v>21.516682090500002</v>
+      </c>
+      <c r="AW38">
+        <v>21.516682090500002</v>
+      </c>
+      <c r="AX38">
+        <v>21.516682090500002</v>
+      </c>
+      <c r="AY38">
+        <v>0</v>
+      </c>
+      <c r="AZ38">
+        <v>0</v>
+      </c>
+      <c r="BA38">
+        <v>0</v>
+      </c>
+      <c r="BB38">
+        <v>0</v>
+      </c>
+      <c r="BC38">
+        <v>0</v>
+      </c>
+      <c r="BD38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2">
         <f t="shared" si="0"/>
@@ -16170,8 +17286,38 @@
       <c r="AT39">
         <v>0.48518</v>
       </c>
-    </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU39">
+        <v>21.239260155</v>
+      </c>
+      <c r="AV39">
+        <v>21.239260155</v>
+      </c>
+      <c r="AW39">
+        <v>21.239260155</v>
+      </c>
+      <c r="AX39">
+        <v>21.239260155</v>
+      </c>
+      <c r="AY39">
+        <v>0</v>
+      </c>
+      <c r="AZ39">
+        <v>0</v>
+      </c>
+      <c r="BA39">
+        <v>0</v>
+      </c>
+      <c r="BB39">
+        <v>0</v>
+      </c>
+      <c r="BC39">
+        <v>0</v>
+      </c>
+      <c r="BD39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2">
         <f t="shared" si="0"/>
@@ -16309,8 +17455,38 @@
       <c r="AT40">
         <v>0.48664499999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU40">
+        <v>20.932572150000002</v>
+      </c>
+      <c r="AV40">
+        <v>20.932572150000002</v>
+      </c>
+      <c r="AW40">
+        <v>20.932572150000002</v>
+      </c>
+      <c r="AX40">
+        <v>20.932572150000002</v>
+      </c>
+      <c r="AY40">
+        <v>0</v>
+      </c>
+      <c r="AZ40">
+        <v>0</v>
+      </c>
+      <c r="BA40">
+        <v>0</v>
+      </c>
+      <c r="BB40">
+        <v>0</v>
+      </c>
+      <c r="BC40">
+        <v>0</v>
+      </c>
+      <c r="BD40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2">
         <f>B40+1</f>
@@ -16448,10 +17624,1675 @@
       <c r="AT41">
         <v>0.529443</v>
       </c>
+      <c r="AU41">
+        <v>20.648072799000001</v>
+      </c>
+      <c r="AV41">
+        <v>20.648072799000001</v>
+      </c>
+      <c r="AW41">
+        <v>20.648072799000001</v>
+      </c>
+      <c r="AX41">
+        <v>20.648072799000001</v>
+      </c>
+      <c r="AY41">
+        <v>0</v>
+      </c>
+      <c r="AZ41">
+        <v>0</v>
+      </c>
+      <c r="BA41">
+        <v>0</v>
+      </c>
+      <c r="BB41">
+        <v>0</v>
+      </c>
+      <c r="BC41">
+        <v>0</v>
+      </c>
+      <c r="BD41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:56" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="Q42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R42" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S42" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T42" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="U42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V42" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="P43" s="2">
+        <v>2022</v>
+      </c>
+      <c r="Q43" s="35">
+        <f>Q3*J3</f>
+        <v>259.11</v>
+      </c>
+      <c r="R43" s="35">
+        <f t="shared" ref="R43:S58" si="1">R3*K3</f>
+        <v>964.9399604370642</v>
+      </c>
+      <c r="S43" s="35">
+        <f t="shared" si="1"/>
+        <v>2075.1380374402711</v>
+      </c>
+      <c r="T43" s="34">
+        <f>Q43/T3</f>
+        <v>0.29129520747377774</v>
+      </c>
+      <c r="U43" s="34">
+        <f t="shared" ref="U43:V43" si="2">R43/U3</f>
+        <v>0.44905365265612646</v>
+      </c>
+      <c r="V43" s="34">
+        <f t="shared" si="2"/>
+        <v>0.46246443438016527</v>
+      </c>
+    </row>
+    <row r="44" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="P44" s="2">
+        <f>P43+1</f>
+        <v>2023</v>
+      </c>
+      <c r="Q44" s="35">
+        <f t="shared" ref="Q44:Q81" si="3">Q4*J4</f>
+        <v>254.91263601848797</v>
+      </c>
+      <c r="R44" s="35">
+        <f t="shared" si="1"/>
+        <v>1010.0899645643754</v>
+      </c>
+      <c r="S44" s="35">
+        <f t="shared" si="1"/>
+        <v>2047.1850828046574</v>
+      </c>
+      <c r="T44" s="34">
+        <f t="shared" ref="T44:T81" si="4">Q44/T4</f>
+        <v>0.28871543969837354</v>
+      </c>
+      <c r="U44" s="34">
+        <f t="shared" ref="U44:U81" si="5">R44/U4</f>
+        <v>0.43719646316379784</v>
+      </c>
+      <c r="V44" s="34">
+        <f t="shared" ref="V44:V81" si="6">S44/V4</f>
+        <v>0.45319277941328406</v>
+      </c>
+    </row>
+    <row r="45" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="P45" s="2">
+        <f t="shared" ref="P45:P80" si="7">P44+1</f>
+        <v>2024</v>
+      </c>
+      <c r="Q45" s="35">
+        <f t="shared" si="3"/>
+        <v>260.39454348547713</v>
+      </c>
+      <c r="R45" s="35">
+        <f t="shared" si="1"/>
+        <v>1047.6108433069578</v>
+      </c>
+      <c r="S45" s="35">
+        <f t="shared" si="1"/>
+        <v>2124.9949512029584</v>
+      </c>
+      <c r="T45" s="34">
+        <f t="shared" si="4"/>
+        <v>0.28888110971441566</v>
+      </c>
+      <c r="U45" s="34">
+        <f t="shared" si="5"/>
+        <v>0.43822638253929302</v>
+      </c>
+      <c r="V45" s="34">
+        <f t="shared" si="6"/>
+        <v>0.45548847797958941</v>
+      </c>
+    </row>
+    <row r="46" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="P46" s="2">
+        <f t="shared" si="7"/>
+        <v>2025</v>
+      </c>
+      <c r="Q46" s="35">
+        <f t="shared" si="3"/>
+        <v>261.2422936968577</v>
+      </c>
+      <c r="R46" s="35">
+        <f t="shared" si="1"/>
+        <v>1083.4383563975152</v>
+      </c>
+      <c r="S46" s="35">
+        <f t="shared" si="1"/>
+        <v>2200.4762546473635</v>
+      </c>
+      <c r="T46" s="34">
+        <f t="shared" si="4"/>
+        <v>0.28315264539773438</v>
+      </c>
+      <c r="U46" s="34">
+        <f t="shared" si="5"/>
+        <v>0.43929706702246896</v>
+      </c>
+      <c r="V46" s="34">
+        <f t="shared" si="6"/>
+        <v>0.45787547122820638</v>
+      </c>
+    </row>
+    <row r="47" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="P47" s="2">
+        <f t="shared" si="7"/>
+        <v>2026</v>
+      </c>
+      <c r="Q47" s="35">
+        <f t="shared" si="3"/>
+        <v>265.1921682738751</v>
+      </c>
+      <c r="R47" s="35">
+        <f t="shared" si="1"/>
+        <v>1118.9882205275837</v>
+      </c>
+      <c r="S47" s="35">
+        <f t="shared" si="1"/>
+        <v>2297.0872814045447</v>
+      </c>
+      <c r="T47" s="34">
+        <f t="shared" si="4"/>
+        <v>0.27919373403576891</v>
+      </c>
+      <c r="U47" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44330761693998993</v>
+      </c>
+      <c r="V47" s="34">
+        <f t="shared" si="6"/>
+        <v>0.45954337116460803</v>
+      </c>
+    </row>
+    <row r="48" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="P48" s="2">
+        <f t="shared" si="7"/>
+        <v>2027</v>
+      </c>
+      <c r="Q48" s="35">
+        <f t="shared" si="3"/>
+        <v>268.82641437414497</v>
+      </c>
+      <c r="R48" s="35">
+        <f t="shared" si="1"/>
+        <v>1158.2729611008319</v>
+      </c>
+      <c r="S48" s="35">
+        <f t="shared" si="1"/>
+        <v>2393.9586317058784</v>
+      </c>
+      <c r="T48" s="34">
+        <f t="shared" si="4"/>
+        <v>0.27596847860032131</v>
+      </c>
+      <c r="U48" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44649077011176286</v>
+      </c>
+      <c r="V48" s="34">
+        <f t="shared" si="6"/>
+        <v>0.46038374277025002</v>
+      </c>
+    </row>
+    <row r="49" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P49" s="2">
+        <f t="shared" si="7"/>
+        <v>2028</v>
+      </c>
+      <c r="Q49" s="35">
+        <f t="shared" si="3"/>
+        <v>271.89912082345342</v>
+      </c>
+      <c r="R49" s="35">
+        <f t="shared" si="1"/>
+        <v>1198.29830385379</v>
+      </c>
+      <c r="S49" s="35">
+        <f t="shared" si="1"/>
+        <v>2489.4083207512108</v>
+      </c>
+      <c r="T49" s="34">
+        <f t="shared" si="4"/>
+        <v>0.27244946875032905</v>
+      </c>
+      <c r="U49" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44895892331149917</v>
+      </c>
+      <c r="V49" s="34">
+        <f t="shared" si="6"/>
+        <v>0.46043622751163121</v>
+      </c>
+    </row>
+    <row r="50" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P50" s="2">
+        <f t="shared" si="7"/>
+        <v>2029</v>
+      </c>
+      <c r="Q50" s="35">
+        <f t="shared" si="3"/>
+        <v>274.85929590395972</v>
+      </c>
+      <c r="R50" s="35">
+        <f t="shared" si="1"/>
+        <v>1238.3305980850496</v>
+      </c>
+      <c r="S50" s="35">
+        <f t="shared" si="1"/>
+        <v>2585.5839068278224</v>
+      </c>
+      <c r="T50" s="34">
+        <f t="shared" si="4"/>
+        <v>0.26865602821253232</v>
+      </c>
+      <c r="U50" s="34">
+        <f t="shared" si="5"/>
+        <v>0.45092513221362235</v>
+      </c>
+      <c r="V50" s="34">
+        <f t="shared" si="6"/>
+        <v>0.45988746539667186</v>
+      </c>
+    </row>
+    <row r="51" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P51" s="2">
+        <f t="shared" si="7"/>
+        <v>2030</v>
+      </c>
+      <c r="Q51" s="35">
+        <f t="shared" si="3"/>
+        <v>276.93146600735008</v>
+      </c>
+      <c r="R51" s="35">
+        <f t="shared" si="1"/>
+        <v>1278.4315801546334</v>
+      </c>
+      <c r="S51" s="35">
+        <f t="shared" si="1"/>
+        <v>2682.7891571617733</v>
+      </c>
+      <c r="T51" s="34">
+        <f t="shared" si="4"/>
+        <v>0.26356101568181178</v>
+      </c>
+      <c r="U51" s="34">
+        <f t="shared" si="5"/>
+        <v>0.45238681944770592</v>
+      </c>
+      <c r="V51" s="34">
+        <f t="shared" si="6"/>
+        <v>0.45899423212284379</v>
+      </c>
+    </row>
+    <row r="52" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P52" s="2">
+        <f t="shared" si="7"/>
+        <v>2031</v>
+      </c>
+      <c r="Q52" s="35">
+        <f t="shared" si="3"/>
+        <v>278.75039329805992</v>
+      </c>
+      <c r="R52" s="35">
+        <f t="shared" si="1"/>
+        <v>1324.0591808195736</v>
+      </c>
+      <c r="S52" s="35">
+        <f t="shared" si="1"/>
+        <v>2778.7632689105144</v>
+      </c>
+      <c r="T52" s="34">
+        <f t="shared" si="4"/>
+        <v>0.257213875502256</v>
+      </c>
+      <c r="U52" s="34">
+        <f t="shared" si="5"/>
+        <v>0.45191121256952388</v>
+      </c>
+      <c r="V52" s="34">
+        <f t="shared" si="6"/>
+        <v>0.45700261477606191</v>
+      </c>
+    </row>
+    <row r="53" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P53" s="2">
+        <f t="shared" si="7"/>
+        <v>2032</v>
+      </c>
+      <c r="Q53" s="35">
+        <f t="shared" si="3"/>
+        <v>281.40204772596178</v>
+      </c>
+      <c r="R53" s="35">
+        <f t="shared" si="1"/>
+        <v>1371.9165246518539</v>
+      </c>
+      <c r="S53" s="35">
+        <f t="shared" si="1"/>
+        <v>2878.4701634420271</v>
+      </c>
+      <c r="T53" s="34">
+        <f t="shared" si="4"/>
+        <v>0.25174407790766035</v>
+      </c>
+      <c r="U53" s="34">
+        <f t="shared" si="5"/>
+        <v>0.45097531800357443</v>
+      </c>
+      <c r="V53" s="34">
+        <f t="shared" si="6"/>
+        <v>0.45476623389967502</v>
+      </c>
+    </row>
+    <row r="54" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P54" s="2">
+        <f t="shared" si="7"/>
+        <v>2033</v>
+      </c>
+      <c r="Q54" s="35">
+        <f t="shared" si="3"/>
+        <v>281.64399023672877</v>
+      </c>
+      <c r="R54" s="35">
+        <f t="shared" si="1"/>
+        <v>1419.6469180060349</v>
+      </c>
+      <c r="S54" s="35">
+        <f t="shared" si="1"/>
+        <v>2975.9453348513812</v>
+      </c>
+      <c r="T54" s="34">
+        <f t="shared" si="4"/>
+        <v>0.24407583735157443</v>
+      </c>
+      <c r="U54" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44979624802168272</v>
+      </c>
+      <c r="V54" s="34">
+        <f t="shared" si="6"/>
+        <v>0.45234763536879036</v>
+      </c>
+    </row>
+    <row r="55" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P55" s="2">
+        <f t="shared" si="7"/>
+        <v>2034</v>
+      </c>
+      <c r="Q55" s="35">
+        <f t="shared" si="3"/>
+        <v>283.8574488188799</v>
+      </c>
+      <c r="R55" s="35">
+        <f t="shared" si="1"/>
+        <v>1468.8365283168321</v>
+      </c>
+      <c r="S55" s="35">
+        <f t="shared" si="1"/>
+        <v>3083.5647468643951</v>
+      </c>
+      <c r="T55" s="34">
+        <f t="shared" si="4"/>
+        <v>0.23790193251496425</v>
+      </c>
+      <c r="U55" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44887525084095764</v>
+      </c>
+      <c r="V55" s="34">
+        <f t="shared" si="6"/>
+        <v>0.45017449598076342</v>
+      </c>
+    </row>
+    <row r="56" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P56" s="2">
+        <f t="shared" si="7"/>
+        <v>2035</v>
+      </c>
+      <c r="Q56" s="35">
+        <f t="shared" si="3"/>
+        <v>284.35085706261134</v>
+      </c>
+      <c r="R56" s="35">
+        <f t="shared" si="1"/>
+        <v>1519.1268578848251</v>
+      </c>
+      <c r="S56" s="35">
+        <f t="shared" si="1"/>
+        <v>3193.5437389989752</v>
+      </c>
+      <c r="T56" s="34">
+        <f t="shared" si="4"/>
+        <v>0.23014856784858992</v>
+      </c>
+      <c r="U56" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44765783347129073</v>
+      </c>
+      <c r="V56" s="34">
+        <f t="shared" si="6"/>
+        <v>0.4480267646553987</v>
+      </c>
+    </row>
+    <row r="57" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P57" s="2">
+        <f t="shared" si="7"/>
+        <v>2036</v>
+      </c>
+      <c r="Q57" s="35">
+        <f t="shared" si="3"/>
+        <v>286.2605804082761</v>
+      </c>
+      <c r="R57" s="35">
+        <f t="shared" si="1"/>
+        <v>1575.4472135591386</v>
+      </c>
+      <c r="S57" s="35">
+        <f t="shared" si="1"/>
+        <v>3318.392820063325</v>
+      </c>
+      <c r="T57" s="34">
+        <f t="shared" si="4"/>
+        <v>0.22323298065121272</v>
+      </c>
+      <c r="U57" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44906157482067965</v>
+      </c>
+      <c r="V57" s="34">
+        <f t="shared" si="6"/>
+        <v>0.44678800682668951</v>
+      </c>
+    </row>
+    <row r="58" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P58" s="2">
+        <f t="shared" si="7"/>
+        <v>2037</v>
+      </c>
+      <c r="Q58" s="35">
+        <f t="shared" si="3"/>
+        <v>288.48872189404159</v>
+      </c>
+      <c r="R58" s="35">
+        <f t="shared" si="1"/>
+        <v>1634.3064387789652</v>
+      </c>
+      <c r="S58" s="35">
+        <f t="shared" si="1"/>
+        <v>3450.1346083547451</v>
+      </c>
+      <c r="T58" s="34">
+        <f t="shared" si="4"/>
+        <v>0.21652622951479836</v>
+      </c>
+      <c r="U58" s="34">
+        <f t="shared" si="5"/>
+        <v>0.45010932212006505</v>
+      </c>
+      <c r="V58" s="34">
+        <f t="shared" si="6"/>
+        <v>0.44554601902145707</v>
+      </c>
+    </row>
+    <row r="59" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P59" s="2">
+        <f t="shared" si="7"/>
+        <v>2038</v>
+      </c>
+      <c r="Q59" s="35">
+        <f t="shared" si="3"/>
+        <v>290.97489789552799</v>
+      </c>
+      <c r="R59" s="35">
+        <f t="shared" ref="R59:R81" si="8">R19*K19</f>
+        <v>1695.0643381701047</v>
+      </c>
+      <c r="S59" s="35">
+        <f t="shared" ref="S59:S81" si="9">S19*L19</f>
+        <v>3587.6051733257937</v>
+      </c>
+      <c r="T59" s="34">
+        <f t="shared" si="4"/>
+        <v>0.21022526959239368</v>
+      </c>
+      <c r="U59" s="34">
+        <f t="shared" si="5"/>
+        <v>0.45084376081720767</v>
+      </c>
+      <c r="V59" s="34">
+        <f t="shared" si="6"/>
+        <v>0.44434049706784662</v>
+      </c>
+    </row>
+    <row r="60" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P60" s="2">
+        <f t="shared" si="7"/>
+        <v>2039</v>
+      </c>
+      <c r="Q60" s="35">
+        <f t="shared" si="3"/>
+        <v>293.69799744105518</v>
+      </c>
+      <c r="R60" s="35">
+        <f t="shared" si="8"/>
+        <v>1757.9180827286609</v>
+      </c>
+      <c r="S60" s="35">
+        <f t="shared" si="9"/>
+        <v>3731.1197448043667</v>
+      </c>
+      <c r="T60" s="34">
+        <f t="shared" si="4"/>
+        <v>0.2041937506977225</v>
+      </c>
+      <c r="U60" s="34">
+        <f t="shared" si="5"/>
+        <v>0.45122490495822787</v>
+      </c>
+      <c r="V60" s="34">
+        <f t="shared" si="6"/>
+        <v>0.44300379762397618</v>
+      </c>
+    </row>
+    <row r="61" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P61" s="2">
+        <f t="shared" si="7"/>
+        <v>2040</v>
+      </c>
+      <c r="Q61" s="35">
+        <f t="shared" si="3"/>
+        <v>296.98740686843996</v>
+      </c>
+      <c r="R61" s="35">
+        <f t="shared" si="8"/>
+        <v>1823.360237069789</v>
+      </c>
+      <c r="S61" s="35">
+        <f t="shared" si="9"/>
+        <v>3881.9870290385593</v>
+      </c>
+      <c r="T61" s="34">
+        <f t="shared" si="4"/>
+        <v>0.19871226773661813</v>
+      </c>
+      <c r="U61" s="34">
+        <f t="shared" si="5"/>
+        <v>0.4513714815996111</v>
+      </c>
+      <c r="V61" s="34">
+        <f t="shared" si="6"/>
+        <v>0.44171212710229951</v>
+      </c>
+    </row>
+    <row r="62" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P62" s="2">
+        <f t="shared" si="7"/>
+        <v>2041</v>
+      </c>
+      <c r="Q62" s="35">
+        <f t="shared" si="3"/>
+        <v>301.23973745605969</v>
+      </c>
+      <c r="R62" s="35">
+        <f t="shared" si="8"/>
+        <v>1892.9433237169328</v>
+      </c>
+      <c r="S62" s="35">
+        <f t="shared" si="9"/>
+        <v>4043.8998312393055</v>
+      </c>
+      <c r="T62" s="34">
+        <f t="shared" si="4"/>
+        <v>0.19355650915356523</v>
+      </c>
+      <c r="U62" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44969753756902647</v>
+      </c>
+      <c r="V62" s="34">
+        <f t="shared" si="6"/>
+        <v>0.43987084524291459</v>
+      </c>
+    </row>
+    <row r="63" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P63" s="2">
+        <f t="shared" si="7"/>
+        <v>2042</v>
+      </c>
+      <c r="Q63" s="35">
+        <f t="shared" si="3"/>
+        <v>305.91931139557641</v>
+      </c>
+      <c r="R63" s="35">
+        <f t="shared" si="8"/>
+        <v>1965.8055832919385</v>
+      </c>
+      <c r="S63" s="35">
+        <f t="shared" si="9"/>
+        <v>4213.071922784583</v>
+      </c>
+      <c r="T63" s="34">
+        <f t="shared" si="4"/>
+        <v>0.18904679919638639</v>
+      </c>
+      <c r="U63" s="34">
+        <f t="shared" si="5"/>
+        <v>0.4479651763306835</v>
+      </c>
+      <c r="V63" s="34">
+        <f t="shared" si="6"/>
+        <v>0.43805855127938187</v>
+      </c>
+    </row>
+    <row r="64" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P64" s="2">
+        <f t="shared" si="7"/>
+        <v>2043</v>
+      </c>
+      <c r="Q64" s="35">
+        <f t="shared" si="3"/>
+        <v>311.61861399555238</v>
+      </c>
+      <c r="R64" s="35">
+        <f t="shared" si="8"/>
+        <v>2040.6442274744611</v>
+      </c>
+      <c r="S64" s="35">
+        <f t="shared" si="9"/>
+        <v>4395.2800142165715</v>
+      </c>
+      <c r="T64" s="34">
+        <f t="shared" si="4"/>
+        <v>0.18525239666110965</v>
+      </c>
+      <c r="U64" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44642691793029649</v>
+      </c>
+      <c r="V64" s="34">
+        <f t="shared" si="6"/>
+        <v>0.43663789519337221</v>
+      </c>
+    </row>
+    <row r="65" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P65" s="2">
+        <f t="shared" si="7"/>
+        <v>2044</v>
+      </c>
+      <c r="Q65" s="35">
+        <f t="shared" si="3"/>
+        <v>318.5445522932668</v>
+      </c>
+      <c r="R65" s="35">
+        <f t="shared" si="8"/>
+        <v>2117.0427666798378</v>
+      </c>
+      <c r="S65" s="35">
+        <f t="shared" si="9"/>
+        <v>4592.282730006611</v>
+      </c>
+      <c r="T65" s="34">
+        <f t="shared" si="4"/>
+        <v>0.1822493648157833</v>
+      </c>
+      <c r="U65" s="34">
+        <f t="shared" si="5"/>
+        <v>0.445271377995549</v>
+      </c>
+      <c r="V65" s="34">
+        <f t="shared" si="6"/>
+        <v>0.4357182247479367</v>
+      </c>
+    </row>
+    <row r="66" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P66" s="2">
+        <f t="shared" si="7"/>
+        <v>2045</v>
+      </c>
+      <c r="Q66" s="35">
+        <f t="shared" si="3"/>
+        <v>326.48209563817477</v>
+      </c>
+      <c r="R66" s="35">
+        <f t="shared" si="8"/>
+        <v>2195.2094410972963</v>
+      </c>
+      <c r="S66" s="35">
+        <f t="shared" si="9"/>
+        <v>4803.0397375448883</v>
+      </c>
+      <c r="T66" s="34">
+        <f t="shared" si="4"/>
+        <v>0.17994736079532539</v>
+      </c>
+      <c r="U66" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44443645794600789</v>
+      </c>
+      <c r="V66" s="34">
+        <f t="shared" si="6"/>
+        <v>0.43531700817831703</v>
+      </c>
+    </row>
+    <row r="67" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P67" s="2">
+        <f t="shared" si="7"/>
+        <v>2046</v>
+      </c>
+      <c r="Q67" s="35">
+        <f t="shared" si="3"/>
+        <v>334.6769471769606</v>
+      </c>
+      <c r="R67" s="35">
+        <f t="shared" si="8"/>
+        <v>2274.3191098577799</v>
+      </c>
+      <c r="S67" s="35">
+        <f t="shared" si="9"/>
+        <v>5016.4559155219658</v>
+      </c>
+      <c r="T67" s="34">
+        <f t="shared" si="4"/>
+        <v>0.17798367732956136</v>
+      </c>
+      <c r="U67" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44396882695800655</v>
+      </c>
+      <c r="V67" s="34">
+        <f t="shared" si="6"/>
+        <v>0.43518916043035794</v>
+      </c>
+    </row>
+    <row r="68" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P68" s="2">
+        <f t="shared" si="7"/>
+        <v>2047</v>
+      </c>
+      <c r="Q68" s="35">
+        <f t="shared" si="3"/>
+        <v>343.64811139298894</v>
+      </c>
+      <c r="R68" s="35">
+        <f t="shared" si="8"/>
+        <v>2356.6488941887751</v>
+      </c>
+      <c r="S68" s="35">
+        <f t="shared" si="9"/>
+        <v>5241.315645886868</v>
+      </c>
+      <c r="T68" s="34">
+        <f t="shared" si="4"/>
+        <v>0.17639624640326715</v>
+      </c>
+      <c r="U68" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44362620931824903</v>
+      </c>
+      <c r="V68" s="34">
+        <f t="shared" si="6"/>
+        <v>0.43524641268332376</v>
+      </c>
+    </row>
+    <row r="69" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P69" s="2">
+        <f t="shared" si="7"/>
+        <v>2048</v>
+      </c>
+      <c r="Q69" s="35">
+        <f t="shared" si="3"/>
+        <v>353.66867887475439</v>
+      </c>
+      <c r="R69" s="35">
+        <f t="shared" si="8"/>
+        <v>2440.5092221895256</v>
+      </c>
+      <c r="S69" s="35">
+        <f t="shared" si="9"/>
+        <v>5478.1233576441409</v>
+      </c>
+      <c r="T69" s="34">
+        <f t="shared" si="4"/>
+        <v>0.17538913298160874</v>
+      </c>
+      <c r="U69" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44356281505282119</v>
+      </c>
+      <c r="V69" s="34">
+        <f t="shared" si="6"/>
+        <v>0.43574451196553421</v>
+      </c>
+    </row>
+    <row r="70" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P70" s="2">
+        <f t="shared" si="7"/>
+        <v>2049</v>
+      </c>
+      <c r="Q70" s="35">
+        <f t="shared" si="3"/>
+        <v>365.05188351612236</v>
+      </c>
+      <c r="R70" s="35">
+        <f t="shared" si="8"/>
+        <v>2524.7987317462871</v>
+      </c>
+      <c r="S70" s="35">
+        <f t="shared" si="9"/>
+        <v>5729.3105745616922</v>
+      </c>
+      <c r="T70" s="34">
+        <f t="shared" si="4"/>
+        <v>0.17504118086430356</v>
+      </c>
+      <c r="U70" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44401433827731335</v>
+      </c>
+      <c r="V70" s="34">
+        <f t="shared" si="6"/>
+        <v>0.43687872255638299</v>
+      </c>
+    </row>
+    <row r="71" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P71" s="2">
+        <f t="shared" si="7"/>
+        <v>2050</v>
+      </c>
+      <c r="Q71" s="35">
+        <f t="shared" si="3"/>
+        <v>377.81674163543528</v>
+      </c>
+      <c r="R71" s="35">
+        <f t="shared" si="8"/>
+        <v>2610.3759614330543</v>
+      </c>
+      <c r="S71" s="35">
+        <f t="shared" si="9"/>
+        <v>5997.8559239861897</v>
+      </c>
+      <c r="T71" s="34">
+        <f t="shared" si="4"/>
+        <v>0.17522423424440112</v>
+      </c>
+      <c r="U71" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44473111467180743</v>
+      </c>
+      <c r="V71" s="34">
+        <f t="shared" si="6"/>
+        <v>0.4384051495924437</v>
+      </c>
+    </row>
+    <row r="72" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P72" s="2">
+        <f t="shared" si="7"/>
+        <v>2051</v>
+      </c>
+      <c r="Q72" s="35">
+        <f t="shared" si="3"/>
+        <v>391.80948002707288</v>
+      </c>
+      <c r="R72" s="35">
+        <f t="shared" si="8"/>
+        <v>2694.7515720275646</v>
+      </c>
+      <c r="S72" s="35">
+        <f t="shared" si="9"/>
+        <v>6290.7229731160742</v>
+      </c>
+      <c r="T72" s="34">
+        <f t="shared" si="4"/>
+        <v>0.17567332189724072</v>
+      </c>
+      <c r="U72" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44568236572933495</v>
+      </c>
+      <c r="V72" s="34">
+        <f t="shared" si="6"/>
+        <v>0.44020344810542356</v>
+      </c>
+    </row>
+    <row r="73" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P73" s="2">
+        <f t="shared" si="7"/>
+        <v>2052</v>
+      </c>
+      <c r="Q73" s="35">
+        <f t="shared" si="3"/>
+        <v>406.09331267195199</v>
+      </c>
+      <c r="R73" s="35">
+        <f t="shared" si="8"/>
+        <v>2781.0414154161754</v>
+      </c>
+      <c r="S73" s="35">
+        <f t="shared" si="9"/>
+        <v>6590.2391454826893</v>
+      </c>
+      <c r="T73" s="34">
+        <f t="shared" si="4"/>
+        <v>0.17620912547977835</v>
+      </c>
+      <c r="U73" s="34">
+        <f t="shared" si="5"/>
+        <v>0.4465119149016798</v>
+      </c>
+      <c r="V73" s="34">
+        <f t="shared" si="6"/>
+        <v>0.44179357294006566</v>
+      </c>
+    </row>
+    <row r="74" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P74" s="2">
+        <f t="shared" si="7"/>
+        <v>2053</v>
+      </c>
+      <c r="Q74" s="35">
+        <f t="shared" si="3"/>
+        <v>421.05562128263341</v>
+      </c>
+      <c r="R74" s="35">
+        <f t="shared" si="8"/>
+        <v>2867.7970930058964</v>
+      </c>
+      <c r="S74" s="35">
+        <f t="shared" si="9"/>
+        <v>6900.8627121885993</v>
+      </c>
+      <c r="T74" s="34">
+        <f t="shared" si="4"/>
+        <v>0.17688216888655975</v>
+      </c>
+      <c r="U74" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44749407324971041</v>
+      </c>
+      <c r="V74" s="34">
+        <f t="shared" si="6"/>
+        <v>0.44342009651140118</v>
+      </c>
+    </row>
+    <row r="75" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P75" s="2">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="Q75" s="35">
+        <f t="shared" si="3"/>
+        <v>436.61682163283137</v>
+      </c>
+      <c r="R75" s="35">
+        <f t="shared" si="8"/>
+        <v>2957.8761307157961</v>
+      </c>
+      <c r="S75" s="35">
+        <f t="shared" si="9"/>
+        <v>7152.2917480789329</v>
+      </c>
+      <c r="T75" s="34">
+        <f t="shared" si="4"/>
+        <v>0.1777480771024155</v>
+      </c>
+      <c r="U75" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44834238706327928</v>
+      </c>
+      <c r="V75" s="34">
+        <f t="shared" si="6"/>
+        <v>0.44264106739968467</v>
+      </c>
+    </row>
+    <row r="76" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P76" s="2">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="Q76" s="35">
+        <f t="shared" si="3"/>
+        <v>453.66982088685688</v>
+      </c>
+      <c r="R76" s="35">
+        <f t="shared" si="8"/>
+        <v>3053.2261294868067</v>
+      </c>
+      <c r="S76" s="35">
+        <f t="shared" si="9"/>
+        <v>7424.1410165369416</v>
+      </c>
+      <c r="T76" s="34">
+        <f t="shared" si="4"/>
+        <v>0.17923112392811982</v>
+      </c>
+      <c r="U76" s="34">
+        <f t="shared" si="5"/>
+        <v>0.44986056231894661</v>
+      </c>
+      <c r="V76" s="34">
+        <f t="shared" si="6"/>
+        <v>0.44328787588515223</v>
+      </c>
+    </row>
+    <row r="77" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P77" s="2">
+        <f t="shared" si="7"/>
+        <v>2056</v>
+      </c>
+      <c r="Q77" s="35">
+        <f t="shared" si="3"/>
+        <v>472.31203963678774</v>
+      </c>
+      <c r="R77" s="35">
+        <f t="shared" si="8"/>
+        <v>3149.9194167185137</v>
+      </c>
+      <c r="S77" s="35">
+        <f t="shared" si="9"/>
+        <v>7732.1366361783248</v>
+      </c>
+      <c r="T77" s="34">
+        <f t="shared" si="4"/>
+        <v>0.18097841558328426</v>
+      </c>
+      <c r="U77" s="34">
+        <f t="shared" si="5"/>
+        <v>0.45206086426468106</v>
+      </c>
+      <c r="V77" s="34">
+        <f t="shared" si="6"/>
+        <v>0.44553380057346337</v>
+      </c>
+    </row>
+    <row r="78" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P78" s="2">
+        <f t="shared" si="7"/>
+        <v>2057</v>
+      </c>
+      <c r="Q78" s="35">
+        <f t="shared" si="3"/>
+        <v>491.72555771262307</v>
+      </c>
+      <c r="R78" s="35">
+        <f t="shared" si="8"/>
+        <v>3248.636742828704</v>
+      </c>
+      <c r="S78" s="35">
+        <f t="shared" si="9"/>
+        <v>8065.3166589607972</v>
+      </c>
+      <c r="T78" s="34">
+        <f t="shared" si="4"/>
+        <v>0.18269776654119241</v>
+      </c>
+      <c r="U78" s="34">
+        <f t="shared" si="5"/>
+        <v>0.45424170525781049</v>
+      </c>
+      <c r="V78" s="34">
+        <f t="shared" si="6"/>
+        <v>0.44812244118857503</v>
+      </c>
+    </row>
+    <row r="79" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P79" s="2">
+        <f t="shared" si="7"/>
+        <v>2058</v>
+      </c>
+      <c r="Q79" s="35">
+        <f t="shared" si="3"/>
+        <v>510.62656286245561</v>
+      </c>
+      <c r="R79" s="35">
+        <f t="shared" si="8"/>
+        <v>3351.0751938313365</v>
+      </c>
+      <c r="S79" s="35">
+        <f t="shared" si="9"/>
+        <v>8409.870216038833</v>
+      </c>
+      <c r="T79" s="34">
+        <f t="shared" si="4"/>
+        <v>0.1839432863337376</v>
+      </c>
+      <c r="U79" s="34">
+        <f t="shared" si="5"/>
+        <v>0.45575993561992517</v>
+      </c>
+      <c r="V79" s="34">
+        <f t="shared" si="6"/>
+        <v>0.45008936183401849</v>
+      </c>
+    </row>
+    <row r="80" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P80" s="2">
+        <f t="shared" si="7"/>
+        <v>2059</v>
+      </c>
+      <c r="Q80" s="35">
+        <f t="shared" si="3"/>
+        <v>528.57277601338319</v>
+      </c>
+      <c r="R80" s="35">
+        <f t="shared" si="8"/>
+        <v>3458.4803282108046</v>
+      </c>
+      <c r="S80" s="35">
+        <f t="shared" si="9"/>
+        <v>8760.9703672653322</v>
+      </c>
+      <c r="T80" s="34">
+        <f t="shared" si="4"/>
+        <v>0.18454206910502724</v>
+      </c>
+      <c r="U80" s="34">
+        <f t="shared" si="5"/>
+        <v>0.45639816571508562</v>
+      </c>
+      <c r="V80" s="34">
+        <f t="shared" si="6"/>
+        <v>0.45099523868005492</v>
+      </c>
+    </row>
+    <row r="81" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P81" s="2">
+        <f>P80+1</f>
+        <v>2060</v>
+      </c>
+      <c r="Q81" s="35">
+        <f t="shared" si="3"/>
+        <v>546.32393510183124</v>
+      </c>
+      <c r="R81" s="35">
+        <f t="shared" si="8"/>
+        <v>3572.5590316957632</v>
+      </c>
+      <c r="S81" s="35">
+        <f t="shared" si="9"/>
+        <v>9129.2562741771981</v>
+      </c>
+      <c r="T81" s="34">
+        <f t="shared" si="4"/>
+        <v>0.18498448714234048</v>
+      </c>
+      <c r="U81" s="34">
+        <f t="shared" si="5"/>
+        <v>0.45633778934285418</v>
+      </c>
+      <c r="V81" s="34">
+        <f t="shared" si="6"/>
+        <v>0.45108832189761078</v>
+      </c>
+    </row>
+    <row r="82" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q82" s="34"/>
+      <c r="R82" s="34"/>
+      <c r="S82" s="34"/>
+    </row>
+    <row r="83" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q83" s="34"/>
+      <c r="R83" s="34"/>
+      <c r="S83" s="34"/>
+    </row>
+    <row r="84" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q84" s="34"/>
+      <c r="R84" s="34"/>
+      <c r="S84" s="34"/>
+    </row>
+    <row r="85" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q85" s="34"/>
+      <c r="R85" s="34"/>
+      <c r="S85" s="34"/>
+    </row>
+    <row r="86" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q86" s="34"/>
+      <c r="R86" s="34"/>
+      <c r="S86" s="34"/>
+    </row>
+    <row r="87" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q87" s="34"/>
+      <c r="R87" s="34"/>
+      <c r="S87" s="34"/>
+    </row>
+    <row r="88" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q88" s="34"/>
+      <c r="R88" s="34"/>
+      <c r="S88" s="34"/>
+    </row>
+    <row r="89" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q89" s="34"/>
+      <c r="R89" s="34"/>
+      <c r="S89" s="34"/>
+    </row>
+    <row r="90" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q90" s="34"/>
+      <c r="R90" s="34"/>
+      <c r="S90" s="34"/>
+    </row>
+    <row r="91" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q91" s="34"/>
+      <c r="R91" s="34"/>
+      <c r="S91" s="34"/>
+    </row>
+    <row r="92" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q92" s="34"/>
+      <c r="R92" s="34"/>
+      <c r="S92" s="34"/>
+    </row>
+    <row r="93" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q93" s="34"/>
+      <c r="R93" s="34"/>
+      <c r="S93" s="34"/>
+    </row>
+    <row r="94" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q94" s="34"/>
+      <c r="R94" s="34"/>
+      <c r="S94" s="34"/>
+    </row>
+    <row r="95" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q95" s="34"/>
+      <c r="R95" s="34"/>
+      <c r="S95" s="34"/>
+    </row>
+    <row r="96" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="Q96" s="34"/>
+      <c r="R96" s="34"/>
+      <c r="S96" s="34"/>
+    </row>
+    <row r="97" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q97" s="34"/>
+      <c r="R97" s="34"/>
+      <c r="S97" s="34"/>
+    </row>
+    <row r="98" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q98" s="34"/>
+      <c r="R98" s="34"/>
+      <c r="S98" s="34"/>
+    </row>
+    <row r="99" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q99" s="34"/>
+      <c r="R99" s="34"/>
+      <c r="S99" s="34"/>
+    </row>
+    <row r="100" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q100" s="34"/>
+      <c r="R100" s="34"/>
+      <c r="S100" s="34"/>
+    </row>
+    <row r="101" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q101" s="34"/>
+      <c r="R101" s="34"/>
+      <c r="S101" s="34"/>
+    </row>
+    <row r="102" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q102" s="34"/>
+      <c r="R102" s="34"/>
+      <c r="S102" s="34"/>
+    </row>
+    <row r="103" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q103" s="34"/>
+      <c r="R103" s="34"/>
+      <c r="S103" s="34"/>
+    </row>
+    <row r="104" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q104" s="34"/>
+      <c r="R104" s="34"/>
+      <c r="S104" s="34"/>
+    </row>
+    <row r="105" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q105" s="34"/>
+      <c r="R105" s="34"/>
+      <c r="S105" s="34"/>
+    </row>
+    <row r="106" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q106" s="34"/>
+      <c r="R106" s="34"/>
+      <c r="S106" s="34"/>
+    </row>
+    <row r="107" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q107" s="34"/>
+      <c r="R107" s="34"/>
+      <c r="S107" s="34"/>
+    </row>
+    <row r="108" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q108" s="34"/>
+      <c r="R108" s="34"/>
+      <c r="S108" s="34"/>
+    </row>
+    <row r="109" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q109" s="34"/>
+      <c r="R109" s="34"/>
+      <c r="S109" s="34"/>
+    </row>
+    <row r="110" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q110" s="34"/>
+      <c r="R110" s="34"/>
+      <c r="S110" s="34"/>
+    </row>
+    <row r="111" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q111" s="34"/>
+      <c r="R111" s="34"/>
+      <c r="S111" s="34"/>
+    </row>
+    <row r="112" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q112" s="34"/>
+      <c r="R112" s="34"/>
+      <c r="S112" s="34"/>
+    </row>
+    <row r="113" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q113" s="34"/>
+      <c r="R113" s="34"/>
+      <c r="S113" s="34"/>
+    </row>
+    <row r="114" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q114" s="34"/>
+      <c r="R114" s="34"/>
+      <c r="S114" s="34"/>
+    </row>
+    <row r="115" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q115" s="34"/>
+      <c r="R115" s="34"/>
+      <c r="S115" s="34"/>
+    </row>
+    <row r="116" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q116" s="34"/>
+      <c r="R116" s="34"/>
+      <c r="S116" s="34"/>
+    </row>
+    <row r="117" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q117" s="34"/>
+      <c r="R117" s="34"/>
+      <c r="S117" s="34"/>
+    </row>
+    <row r="118" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q118" s="34"/>
+      <c r="R118" s="34"/>
+      <c r="S118" s="34"/>
+    </row>
+    <row r="119" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q119" s="34"/>
+      <c r="R119" s="34"/>
+      <c r="S119" s="34"/>
+    </row>
+    <row r="120" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q120" s="34"/>
+      <c r="R120" s="34"/>
+      <c r="S120" s="34"/>
+    </row>
+    <row r="121" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q121" s="34"/>
+      <c r="R121" s="34"/>
+      <c r="S121" s="34"/>
+    </row>
+    <row r="122" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q122" s="34"/>
+      <c r="R122" s="34"/>
+      <c r="S122" s="34"/>
+    </row>
+    <row r="123" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q123" s="34"/>
+      <c r="R123" s="34"/>
+      <c r="S123" s="34"/>
+    </row>
+    <row r="124" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q124" s="34"/>
+      <c r="R124" s="34"/>
+      <c r="S124" s="34"/>
+    </row>
+    <row r="125" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q125" s="34"/>
+      <c r="R125" s="34"/>
+      <c r="S125" s="34"/>
+    </row>
+    <row r="126" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q126" s="34"/>
+      <c r="R126" s="34"/>
+      <c r="S126" s="34"/>
+    </row>
+    <row r="127" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q127" s="34"/>
+      <c r="R127" s="34"/>
+      <c r="S127" s="34"/>
+    </row>
+    <row r="128" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q128" s="34"/>
+      <c r="R128" s="34"/>
+      <c r="S128" s="34"/>
+    </row>
+    <row r="129" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q129" s="34"/>
+      <c r="R129" s="34"/>
+      <c r="S129" s="34"/>
+    </row>
+    <row r="130" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q130" s="34"/>
+      <c r="R130" s="34"/>
+      <c r="S130" s="34"/>
+    </row>
+    <row r="131" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q131" s="34"/>
+      <c r="R131" s="34"/>
+      <c r="S131" s="34"/>
+    </row>
+    <row r="132" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q132" s="34"/>
+      <c r="R132" s="34"/>
+      <c r="S132" s="34"/>
+    </row>
+    <row r="133" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q133" s="34"/>
+      <c r="R133" s="34"/>
+      <c r="S133" s="34"/>
+    </row>
+    <row r="134" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q134" s="34"/>
+      <c r="R134" s="34"/>
+      <c r="S134" s="34"/>
+    </row>
+    <row r="135" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q135" s="34"/>
+      <c r="R135" s="34"/>
+      <c r="S135" s="34"/>
+    </row>
+    <row r="136" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q136" s="34"/>
+      <c r="R136" s="34"/>
+      <c r="S136" s="34"/>
+    </row>
+    <row r="137" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q137" s="34"/>
+      <c r="R137" s="34"/>
+      <c r="S137" s="34"/>
+    </row>
+    <row r="138" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q138" s="34"/>
+      <c r="R138" s="34"/>
+      <c r="S138" s="34"/>
+    </row>
+    <row r="139" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q139" s="34"/>
+      <c r="R139" s="34"/>
+      <c r="S139" s="34"/>
+    </row>
+    <row r="140" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q140" s="34"/>
+      <c r="R140" s="34"/>
+      <c r="S140" s="34"/>
+    </row>
+    <row r="141" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q141" s="34"/>
+      <c r="R141" s="34"/>
+      <c r="S141" s="34"/>
+    </row>
+    <row r="142" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q142" s="34"/>
+      <c r="R142" s="34"/>
+      <c r="S142" s="34"/>
+    </row>
+    <row r="143" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q143" s="34"/>
+      <c r="R143" s="34"/>
+      <c r="S143" s="34"/>
+    </row>
+    <row r="144" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q144" s="34"/>
+      <c r="R144" s="34"/>
+      <c r="S144" s="34"/>
+    </row>
+    <row r="145" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q145" s="34"/>
+      <c r="R145" s="34"/>
+      <c r="S145" s="34"/>
+    </row>
+    <row r="146" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q146" s="34"/>
+      <c r="R146" s="34"/>
+      <c r="S146" s="34"/>
+    </row>
+    <row r="147" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q147" s="34"/>
+      <c r="R147" s="34"/>
+      <c r="S147" s="34"/>
+    </row>
+    <row r="148" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q148" s="34"/>
+      <c r="R148" s="34"/>
+      <c r="S148" s="34"/>
+    </row>
+    <row r="149" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q149" s="34"/>
+      <c r="R149" s="34"/>
+      <c r="S149" s="34"/>
+    </row>
+    <row r="150" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q150" s="34"/>
+      <c r="R150" s="34"/>
+      <c r="S150" s="34"/>
+    </row>
+    <row r="151" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q151" s="34"/>
+      <c r="R151" s="34"/>
+      <c r="S151" s="34"/>
+    </row>
+    <row r="152" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q152" s="34"/>
+      <c r="R152" s="34"/>
+      <c r="S152" s="34"/>
+    </row>
+    <row r="153" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q153" s="34"/>
+      <c r="R153" s="34"/>
+      <c r="S153" s="34"/>
+    </row>
+    <row r="154" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q154" s="34"/>
+      <c r="R154" s="34"/>
+      <c r="S154" s="34"/>
+    </row>
+    <row r="155" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q155" s="34"/>
+      <c r="R155" s="34"/>
+      <c r="S155" s="34"/>
+    </row>
+    <row r="156" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q156" s="34"/>
+      <c r="R156" s="34"/>
+      <c r="S156" s="34"/>
+    </row>
+    <row r="157" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q157" s="34"/>
+      <c r="R157" s="34"/>
+      <c r="S157" s="34"/>
+    </row>
+    <row r="158" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q158" s="34"/>
+      <c r="R158" s="34"/>
+      <c r="S158" s="34"/>
+    </row>
+    <row r="159" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q159" s="34"/>
+      <c r="R159" s="34"/>
+      <c r="S159" s="34"/>
+    </row>
+    <row r="160" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q160" s="34"/>
+      <c r="R160" s="34"/>
+      <c r="S160" s="34"/>
+    </row>
+    <row r="161" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q161" s="34"/>
+      <c r="R161" s="34"/>
+      <c r="S161" s="34"/>
+    </row>
+    <row r="162" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q162" s="34"/>
+      <c r="R162" s="34"/>
+      <c r="S162" s="34"/>
+    </row>
+    <row r="163" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q163" s="34"/>
+      <c r="R163" s="34"/>
+      <c r="S163" s="34"/>
+    </row>
+    <row r="164" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q164" s="34"/>
+      <c r="R164" s="34"/>
+      <c r="S164" s="34"/>
+    </row>
+    <row r="165" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q165" s="34"/>
+      <c r="R165" s="34"/>
+      <c r="S165" s="34"/>
+    </row>
+    <row r="166" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q166" s="34"/>
+      <c r="R166" s="34"/>
+      <c r="S166" s="34"/>
+    </row>
+    <row r="167" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q167" s="34"/>
+      <c r="R167" s="34"/>
+      <c r="S167" s="34"/>
+    </row>
+    <row r="168" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q168" s="34"/>
+      <c r="R168" s="34"/>
+      <c r="S168" s="34"/>
+    </row>
+    <row r="169" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q169" s="34"/>
+      <c r="R169" s="34"/>
+      <c r="S169" s="34"/>
+    </row>
+    <row r="170" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q170" s="34"/>
+      <c r="R170" s="34"/>
+      <c r="S170" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="AK1:AT1"/>
+    <mergeCell ref="AU1:BD1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:P1"/>

</xml_diff>